<commit_message>
Benchmark: updated XLS analyses
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARM-Specific Functions" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,13 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="78">
   <si>
     <t>N</t>
   </si>
@@ -244,6 +244,27 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>N =</t>
+  </si>
+  <si>
+    <t>FRDM-K66F</t>
+  </si>
+  <si>
+    <t>Arduino M0</t>
+  </si>
+  <si>
+    <t>Teensy CMSIS</t>
+  </si>
+  <si>
+    <t>K66 CMSIS</t>
+  </si>
+  <si>
+    <t>FFTs Per second</t>
+  </si>
+  <si>
+    <t>Max Sample Rate for 250 Hz resolution</t>
+  </si>
 </sst>
 </file>
 
@@ -512,7 +533,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Arduino M0 Pro</c:v>
+                  <c:v>Arduino M0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -652,7 +673,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NXP K66</c:v>
+                  <c:v>FRDM-K66F</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -723,11 +744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142675968"/>
-        <c:axId val="142677888"/>
+        <c:axId val="44747392"/>
+        <c:axId val="44749568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142675968"/>
+        <c:axId val="44747392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142677888"/>
+        <c:crossAx val="44749568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -764,7 +785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142677888"/>
+        <c:axId val="44749568"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -796,7 +817,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142675968"/>
+        <c:crossAx val="44747392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,7 +965,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Arduino M0 Pro</c:v>
+                  <c:v>Arduino M0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1084,7 +1105,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NXP K66</c:v>
+                  <c:v>FRDM-K66F</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1155,11 +1176,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143483648"/>
-        <c:axId val="143485568"/>
+        <c:axId val="99126656"/>
+        <c:axId val="99137024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143483648"/>
+        <c:axId val="99126656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,7 +1209,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143485568"/>
+        <c:crossAx val="99137024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1196,7 +1217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143485568"/>
+        <c:axId val="99137024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1228,7 +1249,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143483648"/>
+        <c:crossAx val="99126656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1251,6 +1272,356 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>FFT Performance</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(Bigger</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> is Better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Compare (2)'!$S$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Int16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Compare (2)'!$U$5:$Y$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Arduino M0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Teensy 3.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FRDM-K66F</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy CMSIS</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>K66 CMSIS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Compare (2)'!$U$6:$Y$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>638.9776357827476</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1921.5987701767872</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2865.3295128939826</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7156.1471303850003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14285.714285714286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Compare (2)'!$S$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Int32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Compare (2)'!$U$5:$Y$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Arduino M0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Teensy 3.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FRDM-K66F</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy CMSIS</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>K66 CMSIS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Compare (2)'!$U$7:$Y$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>235.79344494223059</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1006.8465565847764</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1953.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3292.723081988805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6211.1801242236024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Compare (2)'!$S$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Float</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Compare (2)'!$U$5:$Y$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Arduino M0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Teensy 3.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FRDM-K66F</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Teensy CMSIS</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>K66 CMSIS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Compare (2)'!$U$8:$Y$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>81.221572449642622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>350.90181767141553</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4608.294930875576</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>657.56595386517267</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9523.8095238095229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="99167616"/>
+        <c:axId val="99169408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="99167616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99169408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="99169408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>128-pt FFTs per Second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99167616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1353,7 +1724,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Arduino M0 Pro</c:v>
+                  <c:v>Arduino M0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1493,7 +1864,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NXP K66</c:v>
+                  <c:v>FRDM-K66F</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1564,11 +1935,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88401792"/>
-        <c:axId val="88403968"/>
+        <c:axId val="142418304"/>
+        <c:axId val="142420224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88401792"/>
+        <c:axId val="142418304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88403968"/>
+        <c:crossAx val="142420224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1605,7 +1976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88403968"/>
+        <c:axId val="142420224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1638,7 +2009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88401792"/>
+        <c:crossAx val="142418304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1660,7 +2031,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1763,7 +2134,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Arduino M0 Pro</c:v>
+                  <c:v>Arduino M0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1903,7 +2274,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>NXP K66</c:v>
+                  <c:v>FRDM-K66F</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1974,11 +2345,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="88689280"/>
-        <c:axId val="88703744"/>
+        <c:axId val="142472320"/>
+        <c:axId val="142474240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88689280"/>
+        <c:axId val="142472320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,7 +2378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88703744"/>
+        <c:crossAx val="142474240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2015,7 +2386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88703744"/>
+        <c:axId val="142474240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2048,7 +2419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88689280"/>
+        <c:crossAx val="142472320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2070,7 +2441,303 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Compare!$B$6:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Compare!$I$6:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>802</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1674</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4241</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8763</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43329</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.28413429571303589"/>
+                  <c:y val="-8.4835228929717121E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Compare!$B$6:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Compare!$J$6:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>192.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>383.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>993.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15913429571303586"/>
+                  <c:y val="0.21535323709536308"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Compare!$B$6:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Compare!$K$6:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2461</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146554240"/>
+        <c:axId val="146568320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146554240"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146568320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146568320"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146554240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2123,7 +2790,6 @@
         <c:idx val="1"/>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
@@ -2134,13 +2800,22 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="6"/>
+        <c:idx val="2"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="7"/>
+        <c:idx val="3"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="8"/>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -2313,7 +2988,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2322,11 +2996,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100741504"/>
-        <c:axId val="110358528"/>
+        <c:axId val="146782464"/>
+        <c:axId val="146792448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100741504"/>
+        <c:axId val="146782464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2335,7 +3009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110358528"/>
+        <c:crossAx val="146792448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2343,7 +3017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110358528"/>
+        <c:axId val="146792448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2366,21 +3040,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100741504"/>
+        <c:crossAx val="146782464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2406,7 +3078,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2598,11 +3270,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102149504"/>
-        <c:axId val="102442880"/>
+        <c:axId val="45930752"/>
+        <c:axId val="45936640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102149504"/>
+        <c:axId val="45930752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +3283,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102442880"/>
+        <c:crossAx val="45936640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2619,7 +3291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102442880"/>
+        <c:axId val="45936640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2630,14 +3302,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102149504"/>
+        <c:crossAx val="45930752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2729,6 +3400,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2791,6 +3492,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3921,7 +4652,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A5:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" nonAutoSortDefault="1">
@@ -4020,7 +4751,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
+    <chartFormat chart="0" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4032,7 +4763,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
+    <chartFormat chart="0" format="3" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4044,7 +4775,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
+    <chartFormat chart="0" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -4067,7 +4798,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A4:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0" sortType="descending">
@@ -5707,14 +6438,14 @@
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:M17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -7978,10 +8709,997 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Y23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L13" workbookViewId="0">
+      <selection activeCell="X40" sqref="X40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="3" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
+    <col min="8" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C2" t="str">
+        <f>'Arduino Uno'!$C$7</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="H2" t="str">
+        <f>'Arduino Uno'!$C$7</f>
+        <v>KissFFT</v>
+      </c>
+      <c r="M2" t="str">
+        <f>'Arduino Uno'!$C$7</f>
+        <v>KissFFT</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C3" t="str">
+        <f>'Arduino Uno'!$C$6</f>
+        <v>Int16</v>
+      </c>
+      <c r="H3" t="str">
+        <f>'Arduino Uno'!$G$6</f>
+        <v>Int32</v>
+      </c>
+      <c r="M3" t="str">
+        <f>'Arduino Uno'!$K$6</f>
+        <v>Float</v>
+      </c>
+      <c r="S3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="str">
+        <f>C4</f>
+        <v>FFT per sec</v>
+      </c>
+      <c r="M4" t="str">
+        <f>C4</f>
+        <v>FFT per sec</v>
+      </c>
+      <c r="S4" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4">
+        <f>B8</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Arduino Uno'!$C$2</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="D5" t="str">
+        <f>'Arduino M0 Pro'!$C$2</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="E5" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="F5" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+      <c r="H5" t="str">
+        <f>'Arduino Uno'!$C$2</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="I5" t="str">
+        <f>'Arduino M0 Pro'!$C$2</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="J5" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="K5" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+      <c r="M5" t="str">
+        <f>'Arduino Uno'!$C$2</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="N5" t="str">
+        <f>'Arduino M0 Pro'!$C$2</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="O5" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="P5" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+      <c r="T5" t="str">
+        <f>M5</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="U5" t="str">
+        <f>N5</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="V5" t="str">
+        <f>O5</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="W5" t="str">
+        <f>P5</f>
+        <v>FRDM-K66F</v>
+      </c>
+      <c r="X5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>'Arduino Uno'!$B12</f>
+        <v>32</v>
+      </c>
+      <c r="C6" s="16">
+        <f>1000000/Compare!C6</f>
+        <v>200.77096048827497</v>
+      </c>
+      <c r="D6" s="16">
+        <f>1000000/Compare!D6</f>
+        <v>3126.9543464665417</v>
+      </c>
+      <c r="E6" s="16">
+        <f>1000000/Compare!E6</f>
+        <v>9671.1798839458406</v>
+      </c>
+      <c r="F6" s="16">
+        <f>1000000/Compare!F6</f>
+        <v>14492.753623188406</v>
+      </c>
+      <c r="H6" s="16">
+        <f>1000000/Compare!H6</f>
+        <v>79.622905917574357</v>
+      </c>
+      <c r="I6" s="16">
+        <f>1000000/Compare!I6</f>
+        <v>1246.8827930174564</v>
+      </c>
+      <c r="J6" s="16">
+        <f>1000000/Compare!J6</f>
+        <v>5186.7219917012444</v>
+      </c>
+      <c r="K6" s="16">
+        <f>1000000/Compare!K6</f>
+        <v>9803.9215686274511</v>
+      </c>
+      <c r="M6" s="16">
+        <f>1000000/Compare!M6</f>
+        <v>156.78896205707119</v>
+      </c>
+      <c r="N6" s="16">
+        <f>1000000/Compare!N6</f>
+        <v>457.03839122486289</v>
+      </c>
+      <c r="O6" s="16">
+        <f>1000000/Compare!O6</f>
+        <v>2014.5044319097503</v>
+      </c>
+      <c r="P6" s="16">
+        <f>1000000/Compare!P6</f>
+        <v>21276.59574468085</v>
+      </c>
+      <c r="S6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="16">
+        <f>D8</f>
+        <v>638.9776357827476</v>
+      </c>
+      <c r="V6" s="16">
+        <f>E8</f>
+        <v>1921.5987701767872</v>
+      </c>
+      <c r="W6" s="16">
+        <f>F8</f>
+        <v>2865.3295128939826</v>
+      </c>
+      <c r="X6" s="16">
+        <f>E20</f>
+        <v>7156.1471303850003</v>
+      </c>
+      <c r="Y6" s="16">
+        <f>F20</f>
+        <v>14285.714285714286</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>'Arduino Uno'!$B13</f>
+        <v>64</v>
+      </c>
+      <c r="C7" s="16">
+        <f>1000000/Compare!C7</f>
+        <v>98.986379474184361</v>
+      </c>
+      <c r="D7" s="16">
+        <f>1000000/Compare!D7</f>
+        <v>1594.3877551020407</v>
+      </c>
+      <c r="E7" s="16">
+        <f>1000000/Compare!E7</f>
+        <v>4892.3679060665363</v>
+      </c>
+      <c r="F7" s="16">
+        <f>1000000/Compare!F7</f>
+        <v>7352.9411764705883</v>
+      </c>
+      <c r="H7" s="16" t="e">
+        <f>1000000/Compare!H7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="16">
+        <f>1000000/Compare!I7</f>
+        <v>597.37156511350065</v>
+      </c>
+      <c r="J7" s="16">
+        <f>1000000/Compare!J7</f>
+        <v>2606.8821689259644</v>
+      </c>
+      <c r="K7" s="16">
+        <f>1000000/Compare!K7</f>
+        <v>5263.1578947368425</v>
+      </c>
+      <c r="M7" s="16" t="e">
+        <f>1000000/Compare!M7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="16">
+        <f>1000000/Compare!N7</f>
+        <v>198.60973187686196</v>
+      </c>
+      <c r="O7" s="16">
+        <f>1000000/Compare!O7</f>
+        <v>880.28169014084506</v>
+      </c>
+      <c r="P7" s="16">
+        <f>1000000/Compare!P7</f>
+        <v>12658.227848101265</v>
+      </c>
+      <c r="S7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="16">
+        <f>I8</f>
+        <v>235.79344494223059</v>
+      </c>
+      <c r="V7" s="16">
+        <f>J8</f>
+        <v>1006.8465565847764</v>
+      </c>
+      <c r="W7" s="16">
+        <f>K8</f>
+        <v>1953.125</v>
+      </c>
+      <c r="X7" s="16">
+        <f>J20</f>
+        <v>3292.723081988805</v>
+      </c>
+      <c r="Y7" s="16">
+        <f>K20</f>
+        <v>6211.1801242236024</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>'Arduino Uno'!$B14</f>
+        <v>128</v>
+      </c>
+      <c r="C8" s="16" t="e">
+        <f>1000000/Compare!C8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D8" s="16">
+        <f>1000000/Compare!D8</f>
+        <v>638.9776357827476</v>
+      </c>
+      <c r="E8" s="16">
+        <f>1000000/Compare!E8</f>
+        <v>1921.5987701767872</v>
+      </c>
+      <c r="F8" s="16">
+        <f>1000000/Compare!F8</f>
+        <v>2865.3295128939826</v>
+      </c>
+      <c r="H8" s="16" t="e">
+        <f>1000000/Compare!H8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="16">
+        <f>1000000/Compare!I8</f>
+        <v>235.79344494223059</v>
+      </c>
+      <c r="J8" s="16">
+        <f>1000000/Compare!J8</f>
+        <v>1006.8465565847764</v>
+      </c>
+      <c r="K8" s="16">
+        <f>1000000/Compare!K8</f>
+        <v>1953.125</v>
+      </c>
+      <c r="M8" s="16" t="e">
+        <f>1000000/Compare!M8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="16">
+        <f>1000000/Compare!N8</f>
+        <v>81.221572449642622</v>
+      </c>
+      <c r="O8" s="16">
+        <f>1000000/Compare!O8</f>
+        <v>350.90181767141553</v>
+      </c>
+      <c r="P8" s="16">
+        <f>1000000/Compare!P8</f>
+        <v>4608.294930875576</v>
+      </c>
+      <c r="S8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="16">
+        <f>N8</f>
+        <v>81.221572449642622</v>
+      </c>
+      <c r="V8" s="16">
+        <f>O8</f>
+        <v>350.90181767141553</v>
+      </c>
+      <c r="W8" s="16">
+        <f>P8</f>
+        <v>4608.294930875576</v>
+      </c>
+      <c r="X8" s="16">
+        <f>O20</f>
+        <v>657.56595386517267</v>
+      </c>
+      <c r="Y8" s="16">
+        <f>P20</f>
+        <v>9523.8095238095229</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>'Arduino Uno'!$B15</f>
+        <v>256</v>
+      </c>
+      <c r="C9" s="16" t="e">
+        <f>1000000/Compare!C9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D9" s="16">
+        <f>1000000/Compare!D9</f>
+        <v>324.78077297823967</v>
+      </c>
+      <c r="E9" s="16">
+        <f>1000000/Compare!E9</f>
+        <v>970.49689440993779</v>
+      </c>
+      <c r="F9" s="16">
+        <f>1000000/Compare!F9</f>
+        <v>1457.7259475218659</v>
+      </c>
+      <c r="H9" s="16" t="e">
+        <f>1000000/Compare!H9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" s="16">
+        <f>1000000/Compare!I9</f>
+        <v>114.11617026132603</v>
+      </c>
+      <c r="J9" s="16">
+        <f>1000000/Compare!J9</f>
+        <v>506.07287449392715</v>
+      </c>
+      <c r="K9" s="16">
+        <f>1000000/Compare!K9</f>
+        <v>1030.9278350515465</v>
+      </c>
+      <c r="M9" s="16" t="e">
+        <f>1000000/Compare!M9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="16">
+        <f>1000000/Compare!N9</f>
+        <v>36.564408205053198</v>
+      </c>
+      <c r="O9" s="16">
+        <f>1000000/Compare!O9</f>
+        <v>158.83604942977857</v>
+      </c>
+      <c r="P9" s="16">
+        <f>1000000/Compare!P9</f>
+        <v>2695.4177897574123</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>'Arduino Uno'!$B16</f>
+        <v>512</v>
+      </c>
+      <c r="C10" s="16" t="e">
+        <f>1000000/Compare!C10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D10" s="16">
+        <f>1000000/Compare!D10</f>
+        <v>135.080372821829</v>
+      </c>
+      <c r="E10" s="16">
+        <f>1000000/Compare!E10</f>
+        <v>398.72408293460927</v>
+      </c>
+      <c r="F10" s="16">
+        <f>1000000/Compare!F10</f>
+        <v>594.17706476530009</v>
+      </c>
+      <c r="H10" s="16" t="e">
+        <f>1000000/Compare!H10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="16">
+        <f>1000000/Compare!I10</f>
+        <v>47.386627493721271</v>
+      </c>
+      <c r="J10" s="16">
+        <f>1000000/Compare!J10</f>
+        <v>205.84602717167559</v>
+      </c>
+      <c r="K10" s="16">
+        <f>1000000/Compare!K10</f>
+        <v>406.33888663145063</v>
+      </c>
+      <c r="M10" s="16" t="e">
+        <f>1000000/Compare!M10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="16">
+        <f>1000000/Compare!N10</f>
+        <v>15.690704826460804</v>
+      </c>
+      <c r="O10" s="16">
+        <f>1000000/Compare!O10</f>
+        <v>67.015145422865572</v>
+      </c>
+      <c r="P10" s="16">
+        <f>1000000/Compare!P10</f>
+        <v>1019.3679918450561</v>
+      </c>
+      <c r="S10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>'Arduino Uno'!$B17</f>
+        <v>1024</v>
+      </c>
+      <c r="C11" s="16" t="e">
+        <f>1000000/Compare!C11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" s="16">
+        <f>1000000/Compare!D11</f>
+        <v>68.467826968107687</v>
+      </c>
+      <c r="E11" s="16">
+        <f>1000000/Compare!E11</f>
+        <v>201.00502512562815</v>
+      </c>
+      <c r="F11" s="16">
+        <f>1000000/Compare!F11</f>
+        <v>301.56815440289506</v>
+      </c>
+      <c r="H11" s="16" t="e">
+        <f>1000000/Compare!H11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="16">
+        <f>1000000/Compare!I11</f>
+        <v>23.079231000023078</v>
+      </c>
+      <c r="J11" s="16">
+        <f>1000000/Compare!J11</f>
+        <v>103.31645831180907</v>
+      </c>
+      <c r="K11" s="16">
+        <f>1000000/Compare!K11</f>
+        <v>212.40441801189465</v>
+      </c>
+      <c r="M11" s="16" t="e">
+        <f>1000000/Compare!M11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="16">
+        <f>1000000/Compare!N11</f>
+        <v>7.2218330456636499</v>
+      </c>
+      <c r="O11" s="16">
+        <f>1000000/Compare!O11</f>
+        <v>30.998716653130558</v>
+      </c>
+      <c r="P11" s="16">
+        <f>1000000/Compare!P11</f>
+        <v>584.45353594389246</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C14" t="str">
+        <f>'Teensy 3.2'!$E$7</f>
+        <v>CMSIS FFT</v>
+      </c>
+      <c r="E14" t="str">
+        <f>'Teensy 3.2'!E8</f>
+        <v>Radix4</v>
+      </c>
+      <c r="H14" t="str">
+        <f>'Teensy 3.2'!$E$7</f>
+        <v>CMSIS FFT</v>
+      </c>
+      <c r="M14" t="str">
+        <f>'Teensy 3.2'!$E$7</f>
+        <v>CMSIS FFT</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C15" t="str">
+        <f>'Arduino Uno'!$C$6</f>
+        <v>Int16</v>
+      </c>
+      <c r="H15" t="str">
+        <f>'Teensy 3.2'!$H$6</f>
+        <v>Int32</v>
+      </c>
+      <c r="M15" t="str">
+        <f>'Teensy 3.2'!$K$6</f>
+        <v>Float</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="C16" t="str">
+        <f>C4</f>
+        <v>FFT per sec</v>
+      </c>
+      <c r="H16" t="str">
+        <f>C16</f>
+        <v>FFT per sec</v>
+      </c>
+      <c r="M16" t="str">
+        <f>C16</f>
+        <v>FFT per sec</v>
+      </c>
+      <c r="O16" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="P16" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="str">
+        <f>'Arduino Uno'!$C$2</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="D17" t="str">
+        <f>'Arduino M0 Pro'!$C$2</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="E17" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="F17" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+      <c r="H17" t="str">
+        <f>'Arduino Uno'!$C$2</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="I17" t="str">
+        <f>'Arduino M0 Pro'!$C$2</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="J17" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="K17" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+      <c r="M17" t="str">
+        <f>'Arduino Uno'!$C$2</f>
+        <v>Arduino Uno</v>
+      </c>
+      <c r="N17" t="str">
+        <f>'Arduino M0 Pro'!$C$2</f>
+        <v>Arduino M0</v>
+      </c>
+      <c r="O17" t="str">
+        <f>'Teensy 3.2'!$C$2</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="P17" t="str">
+        <f>'NXP K66'!$C$2</f>
+        <v>FRDM-K66F</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>'Teensy 3.2'!B12</f>
+        <v>32</v>
+      </c>
+      <c r="C18" s="16" t="e">
+        <f>1000000/Compare!C18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D18" s="16" t="e">
+        <f>1000000/Compare!D18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="16">
+        <f>1000000/Compare!E18</f>
+        <v>30864.1975308642</v>
+      </c>
+      <c r="F18" s="16">
+        <f>1000000/Compare!F18</f>
+        <v>58823.529411764706</v>
+      </c>
+      <c r="H18" s="16" t="e">
+        <f>1000000/Compare!H18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="16" t="e">
+        <f>1000000/Compare!I18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="16">
+        <f>1000000/Compare!J18</f>
+        <v>16474.464579901152</v>
+      </c>
+      <c r="K18" s="16">
+        <f>1000000/Compare!K18</f>
+        <v>31250</v>
+      </c>
+      <c r="M18" s="16" t="e">
+        <f>1000000/Compare!M18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="16" t="e">
+        <f>1000000/Compare!N18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="16">
+        <f>1000000/Compare!O18</f>
+        <v>3542.3308537017356</v>
+      </c>
+      <c r="P18" s="16">
+        <f>1000000/Compare!P18</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f>'Teensy 3.2'!B13</f>
+        <v>64</v>
+      </c>
+      <c r="C19" s="16" t="e">
+        <f>1000000/Compare!C19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" s="16" t="e">
+        <f>1000000/Compare!D19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="16">
+        <f>1000000/Compare!E19</f>
+        <v>16528.92561983471</v>
+      </c>
+      <c r="F19" s="16">
+        <f>1000000/Compare!F19</f>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="H19" s="16" t="e">
+        <f>1000000/Compare!H19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="16" t="e">
+        <f>1000000/Compare!I19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" s="16">
+        <f>1000000/Compare!J19</f>
+        <v>8577.8006519128503</v>
+      </c>
+      <c r="K19" s="16">
+        <f>1000000/Compare!K19</f>
+        <v>16666.666666666668</v>
+      </c>
+      <c r="M19" s="16" t="e">
+        <f>1000000/Compare!M19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="16" t="e">
+        <f>1000000/Compare!N19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="16">
+        <f>1000000/Compare!O19</f>
+        <v>1811.4629374682995</v>
+      </c>
+      <c r="P19" s="16">
+        <f>1000000/Compare!P19</f>
+        <v>21276.59574468085</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>'Teensy 3.2'!B14</f>
+        <v>128</v>
+      </c>
+      <c r="C20" s="16" t="e">
+        <f>1000000/Compare!C20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D20" s="16" t="e">
+        <f>1000000/Compare!D20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E20" s="16">
+        <f>1000000/Compare!E20</f>
+        <v>7156.1471303850003</v>
+      </c>
+      <c r="F20" s="16">
+        <f>1000000/Compare!F20</f>
+        <v>14285.714285714286</v>
+      </c>
+      <c r="H20" s="16" t="e">
+        <f>1000000/Compare!H20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I20" s="16" t="e">
+        <f>1000000/Compare!I20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J20" s="16">
+        <f>1000000/Compare!J20</f>
+        <v>3292.723081988805</v>
+      </c>
+      <c r="K20" s="16">
+        <f>1000000/Compare!K20</f>
+        <v>6211.1801242236024</v>
+      </c>
+      <c r="M20" s="16" t="e">
+        <f>1000000/Compare!M20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="16" t="e">
+        <f>1000000/Compare!N20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="16">
+        <f>1000000/Compare!O20</f>
+        <v>657.56595386517267</v>
+      </c>
+      <c r="P20" s="16">
+        <f>1000000/Compare!P20</f>
+        <v>9523.8095238095229</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f>'Teensy 3.2'!B15</f>
+        <v>256</v>
+      </c>
+      <c r="C21" s="16" t="e">
+        <f>1000000/Compare!C21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D21" s="16" t="e">
+        <f>1000000/Compare!D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" s="16">
+        <f>1000000/Compare!E21</f>
+        <v>3669.1861745064944</v>
+      </c>
+      <c r="F21" s="16">
+        <f>1000000/Compare!F21</f>
+        <v>7352.9411764705883</v>
+      </c>
+      <c r="H21" s="16" t="e">
+        <f>1000000/Compare!H21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" s="16" t="e">
+        <f>1000000/Compare!I21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" s="16">
+        <f>1000000/Compare!J21</f>
+        <v>1674.817444898506</v>
+      </c>
+      <c r="K21" s="16">
+        <f>1000000/Compare!K21</f>
+        <v>3154.5741324921137</v>
+      </c>
+      <c r="M21" s="16" t="e">
+        <f>1000000/Compare!M21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" s="16" t="e">
+        <f>1000000/Compare!N21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="16">
+        <f>1000000/Compare!O21</f>
+        <v>330.84975450948218</v>
+      </c>
+      <c r="P21" s="16">
+        <f>1000000/Compare!P21</f>
+        <v>4878.0487804878048</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f>'Teensy 3.2'!B16</f>
+        <v>512</v>
+      </c>
+      <c r="C22" s="16" t="e">
+        <f>1000000/Compare!C22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D22" s="16" t="e">
+        <f>1000000/Compare!D22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22" s="16">
+        <f>1000000/Compare!E22</f>
+        <v>1574.6543633672411</v>
+      </c>
+      <c r="F22" s="16">
+        <f>1000000/Compare!F22</f>
+        <v>3225.8064516129034</v>
+      </c>
+      <c r="H22" s="16" t="e">
+        <f>1000000/Compare!H22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" s="16" t="e">
+        <f>1000000/Compare!I22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" s="16">
+        <f>1000000/Compare!J22</f>
+        <v>677.43334055928892</v>
+      </c>
+      <c r="K22" s="16">
+        <f>1000000/Compare!K22</f>
+        <v>1272.2646310432569</v>
+      </c>
+      <c r="M22" s="16" t="e">
+        <f>1000000/Compare!M22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" s="16" t="e">
+        <f>1000000/Compare!N22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="16">
+        <f>1000000/Compare!O22</f>
+        <v>129.6798205231284</v>
+      </c>
+      <c r="P22" s="16">
+        <f>1000000/Compare!P22</f>
+        <v>2123.1422505307855</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>'Teensy 3.2'!B17</f>
+        <v>1024</v>
+      </c>
+      <c r="C23" s="16" t="e">
+        <f>1000000/Compare!C23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" s="16" t="e">
+        <f>1000000/Compare!D23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="16">
+        <f>1000000/Compare!E23</f>
+        <v>797.19387755102036</v>
+      </c>
+      <c r="F23" s="16">
+        <f>1000000/Compare!F23</f>
+        <v>1628.6644951140065</v>
+      </c>
+      <c r="H23" s="16" t="e">
+        <f>1000000/Compare!H23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="16" t="e">
+        <f>1000000/Compare!I23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" s="16">
+        <f>1000000/Compare!J23</f>
+        <v>342.43291739148299</v>
+      </c>
+      <c r="K23" s="16">
+        <f>1000000/Compare!K23</f>
+        <v>641.84852374839534</v>
+      </c>
+      <c r="M23" s="16" t="e">
+        <f>1000000/Compare!M23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="16" t="e">
+        <f>1000000/Compare!N23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="16">
+        <f>1000000/Compare!O23</f>
+        <v>65.006910234557935</v>
+      </c>
+      <c r="P23" s="16">
+        <f>1000000/Compare!P23</f>
+        <v>1077.5862068965516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8023,15 +9741,15 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H4" t="str">
         <f>C4</f>
-        <v>FFT per sec</v>
+        <v>usec per FFT</v>
       </c>
       <c r="M4" t="str">
         <f>C4</f>
-        <v>FFT per sec</v>
+        <v>usec per FFT</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -8044,7 +9762,7 @@
       </c>
       <c r="D5" t="str">
         <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
+        <v>Arduino M0</v>
       </c>
       <c r="E5" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8052,7 +9770,7 @@
       </c>
       <c r="F5" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
       <c r="H5" t="str">
         <f>'Arduino Uno'!$C$2</f>
@@ -8060,7 +9778,7 @@
       </c>
       <c r="I5" t="str">
         <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
+        <v>Arduino M0</v>
       </c>
       <c r="J5" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8068,7 +9786,7 @@
       </c>
       <c r="K5" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
       <c r="M5" t="str">
         <f>'Arduino Uno'!$C$2</f>
@@ -8076,7 +9794,7 @@
       </c>
       <c r="N5" t="str">
         <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
+        <v>Arduino M0</v>
       </c>
       <c r="O5" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8084,7 +9802,7 @@
       </c>
       <c r="P5" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -8093,52 +9811,52 @@
         <v>32</v>
       </c>
       <c r="C6" s="16">
-        <f>1000000/Compare!C6</f>
-        <v>200.77096048827497</v>
+        <f>'Arduino Uno'!$C12</f>
+        <v>4980.8</v>
       </c>
       <c r="D6" s="16">
-        <f>1000000/Compare!D6</f>
-        <v>3126.9543464665417</v>
+        <f>'Arduino M0 Pro'!C12</f>
+        <v>319.8</v>
       </c>
       <c r="E6" s="16">
-        <f>1000000/Compare!E6</f>
-        <v>9671.1798839458406</v>
+        <f>'Teensy 3.2'!C12</f>
+        <v>103.4</v>
       </c>
       <c r="F6" s="16">
-        <f>1000000/Compare!F6</f>
-        <v>14492.753623188406</v>
+        <f>'NXP K66'!C12</f>
+        <v>69</v>
       </c>
       <c r="H6" s="16">
-        <f>1000000/Compare!H6</f>
-        <v>79.622905917574357</v>
+        <f>'Arduino Uno'!G12</f>
+        <v>12559.2</v>
       </c>
       <c r="I6" s="16">
-        <f>1000000/Compare!I6</f>
-        <v>1246.8827930174564</v>
+        <f>'Arduino M0 Pro'!G12</f>
+        <v>802</v>
       </c>
       <c r="J6" s="16">
-        <f>1000000/Compare!J6</f>
-        <v>5186.7219917012444</v>
+        <f>'Teensy 3.2'!G12</f>
+        <v>192.8</v>
       </c>
       <c r="K6" s="16">
-        <f>1000000/Compare!K6</f>
-        <v>9803.9215686274511</v>
+        <f>'NXP K66'!G12</f>
+        <v>102</v>
       </c>
       <c r="M6" s="16">
-        <f>1000000/Compare!M6</f>
-        <v>156.78896205707119</v>
+        <f>'Arduino Uno'!K12</f>
+        <v>6378</v>
       </c>
       <c r="N6" s="16">
-        <f>1000000/Compare!N6</f>
-        <v>457.03839122486289</v>
+        <f>'Arduino M0 Pro'!K12</f>
+        <v>2188</v>
       </c>
       <c r="O6" s="16">
-        <f>1000000/Compare!O6</f>
-        <v>2014.5044319097503</v>
+        <f>'Teensy 3.2'!K12</f>
+        <v>496.4</v>
       </c>
       <c r="P6" s="16">
-        <f>1000000/Compare!P6</f>
-        <v>21276.59574468085</v>
+        <f>'NXP K66'!K12</f>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -8147,52 +9865,46 @@
         <v>64</v>
       </c>
       <c r="C7" s="16">
-        <f>1000000/Compare!C7</f>
-        <v>98.986379474184361</v>
+        <f>'Arduino Uno'!$C13</f>
+        <v>10102.4</v>
       </c>
       <c r="D7" s="16">
-        <f>1000000/Compare!D7</f>
-        <v>1594.3877551020407</v>
+        <f>'Arduino M0 Pro'!C13</f>
+        <v>627.20000000000005</v>
       </c>
       <c r="E7" s="16">
-        <f>1000000/Compare!E7</f>
-        <v>4892.3679060665363</v>
+        <f>'Teensy 3.2'!C13</f>
+        <v>204.4</v>
       </c>
       <c r="F7" s="16">
-        <f>1000000/Compare!F7</f>
-        <v>7352.9411764705883</v>
-      </c>
-      <c r="H7" s="16" t="e">
-        <f>1000000/Compare!H7</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!C13</f>
+        <v>136</v>
+      </c>
+      <c r="H7" s="16"/>
       <c r="I7" s="16">
-        <f>1000000/Compare!I7</f>
-        <v>597.37156511350065</v>
+        <f>'Arduino M0 Pro'!G13</f>
+        <v>1674</v>
       </c>
       <c r="J7" s="16">
-        <f>1000000/Compare!J7</f>
-        <v>2606.8821689259644</v>
+        <f>'Teensy 3.2'!G13</f>
+        <v>383.6</v>
       </c>
       <c r="K7" s="16">
-        <f>1000000/Compare!K7</f>
-        <v>5263.1578947368425</v>
-      </c>
-      <c r="M7" s="16" t="e">
-        <f>1000000/Compare!M7</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!G13</f>
+        <v>190</v>
+      </c>
+      <c r="M7" s="16"/>
       <c r="N7" s="16">
-        <f>1000000/Compare!N7</f>
-        <v>198.60973187686196</v>
+        <f>'Arduino M0 Pro'!K13</f>
+        <v>5035</v>
       </c>
       <c r="O7" s="16">
-        <f>1000000/Compare!O7</f>
-        <v>880.28169014084506</v>
+        <f>'Teensy 3.2'!K13</f>
+        <v>1136</v>
       </c>
       <c r="P7" s="16">
-        <f>1000000/Compare!P7</f>
-        <v>12658.227848101265</v>
+        <f>'NXP K66'!K13</f>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -8200,53 +9912,44 @@
         <f>'Arduino Uno'!$B14</f>
         <v>128</v>
       </c>
-      <c r="C8" s="16" t="e">
-        <f>1000000/Compare!C8</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C8" s="16"/>
       <c r="D8" s="16">
-        <f>1000000/Compare!D8</f>
-        <v>638.9776357827476</v>
+        <f>'Arduino M0 Pro'!C14</f>
+        <v>1565</v>
       </c>
       <c r="E8" s="16">
-        <f>1000000/Compare!E8</f>
-        <v>1921.5987701767872</v>
+        <f>'Teensy 3.2'!C14</f>
+        <v>520.4</v>
       </c>
       <c r="F8" s="16">
-        <f>1000000/Compare!F8</f>
-        <v>2865.3295128939826</v>
-      </c>
-      <c r="H8" s="16" t="e">
-        <f>1000000/Compare!H8</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!C14</f>
+        <v>349</v>
+      </c>
+      <c r="H8" s="16"/>
       <c r="I8" s="16">
-        <f>1000000/Compare!I8</f>
-        <v>235.79344494223059</v>
+        <f>'Arduino M0 Pro'!G14</f>
+        <v>4241</v>
       </c>
       <c r="J8" s="16">
-        <f>1000000/Compare!J8</f>
-        <v>1006.8465565847764</v>
+        <f>'Teensy 3.2'!G14</f>
+        <v>993.2</v>
       </c>
       <c r="K8" s="16">
-        <f>1000000/Compare!K8</f>
-        <v>1953.125</v>
-      </c>
-      <c r="M8" s="16" t="e">
-        <f>1000000/Compare!M8</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!G14</f>
+        <v>512</v>
+      </c>
+      <c r="M8" s="16"/>
       <c r="N8" s="16">
-        <f>1000000/Compare!N8</f>
-        <v>81.221572449642622</v>
+        <f>'Arduino M0 Pro'!K14</f>
+        <v>12312</v>
       </c>
       <c r="O8" s="16">
-        <f>1000000/Compare!O8</f>
-        <v>350.90181767141553</v>
+        <f>'Teensy 3.2'!K14</f>
+        <v>2849.8</v>
       </c>
       <c r="P8" s="16">
-        <f>1000000/Compare!P8</f>
-        <v>4608.294930875576</v>
+        <f>'NXP K66'!K14</f>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
@@ -8254,53 +9957,44 @@
         <f>'Arduino Uno'!$B15</f>
         <v>256</v>
       </c>
-      <c r="C9" s="16" t="e">
-        <f>1000000/Compare!C9</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C9" s="16"/>
       <c r="D9" s="16">
-        <f>1000000/Compare!D9</f>
-        <v>324.78077297823967</v>
+        <f>'Arduino M0 Pro'!C15</f>
+        <v>3079</v>
       </c>
       <c r="E9" s="16">
-        <f>1000000/Compare!E9</f>
-        <v>970.49689440993779</v>
+        <f>'Teensy 3.2'!C15</f>
+        <v>1030.4000000000001</v>
       </c>
       <c r="F9" s="16">
-        <f>1000000/Compare!F9</f>
-        <v>1457.7259475218659</v>
-      </c>
-      <c r="H9" s="16" t="e">
-        <f>1000000/Compare!H9</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!C15</f>
+        <v>686</v>
+      </c>
+      <c r="H9" s="16"/>
       <c r="I9" s="16">
-        <f>1000000/Compare!I9</f>
-        <v>114.11617026132603</v>
+        <f>'Arduino M0 Pro'!G15</f>
+        <v>8763</v>
       </c>
       <c r="J9" s="16">
-        <f>1000000/Compare!J9</f>
-        <v>506.07287449392715</v>
+        <f>'Teensy 3.2'!G15</f>
+        <v>1976</v>
       </c>
       <c r="K9" s="16">
-        <f>1000000/Compare!K9</f>
-        <v>1030.9278350515465</v>
-      </c>
-      <c r="M9" s="16" t="e">
-        <f>1000000/Compare!M9</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!G15</f>
+        <v>970</v>
+      </c>
+      <c r="M9" s="16"/>
       <c r="N9" s="16">
-        <f>1000000/Compare!N9</f>
-        <v>36.564408205053198</v>
+        <f>'Arduino M0 Pro'!K15</f>
+        <v>27349</v>
       </c>
       <c r="O9" s="16">
-        <f>1000000/Compare!O9</f>
-        <v>158.83604942977857</v>
+        <f>'Teensy 3.2'!K15</f>
+        <v>6295.8</v>
       </c>
       <c r="P9" s="16">
-        <f>1000000/Compare!P9</f>
-        <v>2695.4177897574123</v>
+        <f>'NXP K66'!K15</f>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -8308,53 +10002,44 @@
         <f>'Arduino Uno'!$B16</f>
         <v>512</v>
       </c>
-      <c r="C10" s="16" t="e">
-        <f>1000000/Compare!C10</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C10" s="16"/>
       <c r="D10" s="16">
-        <f>1000000/Compare!D10</f>
-        <v>135.080372821829</v>
+        <f>'Arduino M0 Pro'!C16</f>
+        <v>7403</v>
       </c>
       <c r="E10" s="16">
-        <f>1000000/Compare!E10</f>
-        <v>398.72408293460927</v>
+        <f>'Teensy 3.2'!C16</f>
+        <v>2508</v>
       </c>
       <c r="F10" s="16">
-        <f>1000000/Compare!F10</f>
-        <v>594.17706476530009</v>
-      </c>
-      <c r="H10" s="16" t="e">
-        <f>1000000/Compare!H10</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!C16</f>
+        <v>1683</v>
+      </c>
+      <c r="H10" s="16"/>
       <c r="I10" s="16">
-        <f>1000000/Compare!I10</f>
-        <v>47.386627493721271</v>
+        <f>'Arduino M0 Pro'!G16</f>
+        <v>21103</v>
       </c>
       <c r="J10" s="16">
-        <f>1000000/Compare!J10</f>
-        <v>205.84602717167559</v>
+        <f>'Teensy 3.2'!G16</f>
+        <v>4858</v>
       </c>
       <c r="K10" s="16">
-        <f>1000000/Compare!K10</f>
-        <v>406.33888663145063</v>
-      </c>
-      <c r="M10" s="16" t="e">
-        <f>1000000/Compare!M10</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!G16</f>
+        <v>2461</v>
+      </c>
+      <c r="M10" s="16"/>
       <c r="N10" s="16">
-        <f>1000000/Compare!N10</f>
-        <v>15.690704826460804</v>
+        <f>'Arduino M0 Pro'!K16</f>
+        <v>63732</v>
       </c>
       <c r="O10" s="16">
-        <f>1000000/Compare!O10</f>
-        <v>67.015145422865572</v>
+        <f>'Teensy 3.2'!K16</f>
+        <v>14922</v>
       </c>
       <c r="P10" s="16">
-        <f>1000000/Compare!P10</f>
-        <v>1019.3679918450561</v>
+        <f>'NXP K66'!K16</f>
+        <v>981</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -8362,53 +10047,44 @@
         <f>'Arduino Uno'!$B17</f>
         <v>1024</v>
       </c>
-      <c r="C11" s="16" t="e">
-        <f>1000000/Compare!C11</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C11" s="16"/>
       <c r="D11" s="16">
-        <f>1000000/Compare!D11</f>
-        <v>68.467826968107687</v>
+        <f>'Arduino M0 Pro'!C17</f>
+        <v>14605.4</v>
       </c>
       <c r="E11" s="16">
-        <f>1000000/Compare!E11</f>
-        <v>201.00502512562815</v>
+        <f>'Teensy 3.2'!C17</f>
+        <v>4975</v>
       </c>
       <c r="F11" s="16">
-        <f>1000000/Compare!F11</f>
-        <v>301.56815440289506</v>
-      </c>
-      <c r="H11" s="16" t="e">
-        <f>1000000/Compare!H11</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!C17</f>
+        <v>3316</v>
+      </c>
+      <c r="H11" s="16"/>
       <c r="I11" s="16">
-        <f>1000000/Compare!I11</f>
-        <v>23.079231000023078</v>
+        <f>'Arduino M0 Pro'!G17</f>
+        <v>43329</v>
       </c>
       <c r="J11" s="16">
-        <f>1000000/Compare!J11</f>
-        <v>103.31645831180907</v>
+        <f>'Teensy 3.2'!G17</f>
+        <v>9679</v>
       </c>
       <c r="K11" s="16">
-        <f>1000000/Compare!K11</f>
-        <v>212.40441801189465</v>
-      </c>
-      <c r="M11" s="16" t="e">
-        <f>1000000/Compare!M11</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>'NXP K66'!G17</f>
+        <v>4708</v>
+      </c>
+      <c r="M11" s="16"/>
       <c r="N11" s="16">
-        <f>1000000/Compare!N11</f>
-        <v>7.2218330456636499</v>
+        <f>'Arduino M0 Pro'!K17</f>
+        <v>138469</v>
       </c>
       <c r="O11" s="16">
-        <f>1000000/Compare!O11</f>
-        <v>30.998716653130558</v>
+        <f>'Teensy 3.2'!K17</f>
+        <v>32259.4</v>
       </c>
       <c r="P11" s="16">
-        <f>1000000/Compare!P11</f>
-        <v>584.45353594389246</v>
+        <f>'NXP K66'!K17</f>
+        <v>1711</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -8444,17 +10120,16 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C16" t="str">
-        <f>C4</f>
-        <v>FFT per sec</v>
+      <c r="C16" t="s">
+        <v>57</v>
       </c>
       <c r="H16" t="str">
         <f>C16</f>
-        <v>FFT per sec</v>
+        <v>usec per FFT</v>
       </c>
       <c r="M16" t="str">
         <f>C16</f>
-        <v>FFT per sec</v>
+        <v>usec per FFT</v>
       </c>
       <c r="O16" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8462,7 +10137,7 @@
       </c>
       <c r="P16" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
@@ -8475,7 +10150,7 @@
       </c>
       <c r="D17" t="str">
         <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
+        <v>Arduino M0</v>
       </c>
       <c r="E17" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8483,7 +10158,7 @@
       </c>
       <c r="F17" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
       <c r="H17" t="str">
         <f>'Arduino Uno'!$C$2</f>
@@ -8491,7 +10166,7 @@
       </c>
       <c r="I17" t="str">
         <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
+        <v>Arduino M0</v>
       </c>
       <c r="J17" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8499,7 +10174,7 @@
       </c>
       <c r="K17" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
       <c r="M17" t="str">
         <f>'Arduino Uno'!$C$2</f>
@@ -8507,7 +10182,7 @@
       </c>
       <c r="N17" t="str">
         <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
+        <v>Arduino M0</v>
       </c>
       <c r="O17" t="str">
         <f>'Teensy 3.2'!$C$2</f>
@@ -8515,836 +10190,7 @@
       </c>
       <c r="P17" t="str">
         <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f>'Teensy 3.2'!B12</f>
-        <v>32</v>
-      </c>
-      <c r="C18" s="16" t="e">
-        <f>1000000/Compare!C18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D18" s="16" t="e">
-        <f>1000000/Compare!D18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="16">
-        <f>1000000/Compare!E18</f>
-        <v>30864.1975308642</v>
-      </c>
-      <c r="F18" s="16">
-        <f>1000000/Compare!F18</f>
-        <v>58823.529411764706</v>
-      </c>
-      <c r="H18" s="16" t="e">
-        <f>1000000/Compare!H18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="16" t="e">
-        <f>1000000/Compare!I18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="16">
-        <f>1000000/Compare!J18</f>
-        <v>16474.464579901152</v>
-      </c>
-      <c r="K18" s="16">
-        <f>1000000/Compare!K18</f>
-        <v>31250</v>
-      </c>
-      <c r="M18" s="16" t="e">
-        <f>1000000/Compare!M18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="16" t="e">
-        <f>1000000/Compare!N18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="16">
-        <f>1000000/Compare!O18</f>
-        <v>3542.3308537017356</v>
-      </c>
-      <c r="P18" s="16">
-        <f>1000000/Compare!P18</f>
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f>'Teensy 3.2'!B13</f>
-        <v>64</v>
-      </c>
-      <c r="C19" s="16" t="e">
-        <f>1000000/Compare!C19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D19" s="16" t="e">
-        <f>1000000/Compare!D19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="16">
-        <f>1000000/Compare!E19</f>
-        <v>16528.92561983471</v>
-      </c>
-      <c r="F19" s="16">
-        <f>1000000/Compare!F19</f>
-        <v>33333.333333333336</v>
-      </c>
-      <c r="H19" s="16" t="e">
-        <f>1000000/Compare!H19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="16" t="e">
-        <f>1000000/Compare!I19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J19" s="16">
-        <f>1000000/Compare!J19</f>
-        <v>8577.8006519128503</v>
-      </c>
-      <c r="K19" s="16">
-        <f>1000000/Compare!K19</f>
-        <v>16666.666666666668</v>
-      </c>
-      <c r="M19" s="16" t="e">
-        <f>1000000/Compare!M19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="16" t="e">
-        <f>1000000/Compare!N19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O19" s="16">
-        <f>1000000/Compare!O19</f>
-        <v>1811.4629374682995</v>
-      </c>
-      <c r="P19" s="16">
-        <f>1000000/Compare!P19</f>
-        <v>21276.59574468085</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <f>'Teensy 3.2'!B14</f>
-        <v>128</v>
-      </c>
-      <c r="C20" s="16" t="e">
-        <f>1000000/Compare!C20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D20" s="16" t="e">
-        <f>1000000/Compare!D20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="16">
-        <f>1000000/Compare!E20</f>
-        <v>7156.1471303850003</v>
-      </c>
-      <c r="F20" s="16">
-        <f>1000000/Compare!F20</f>
-        <v>14285.714285714286</v>
-      </c>
-      <c r="H20" s="16" t="e">
-        <f>1000000/Compare!H20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I20" s="16" t="e">
-        <f>1000000/Compare!I20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J20" s="16">
-        <f>1000000/Compare!J20</f>
-        <v>3292.723081988805</v>
-      </c>
-      <c r="K20" s="16">
-        <f>1000000/Compare!K20</f>
-        <v>6211.1801242236024</v>
-      </c>
-      <c r="M20" s="16" t="e">
-        <f>1000000/Compare!M20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" s="16" t="e">
-        <f>1000000/Compare!N20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O20" s="16">
-        <f>1000000/Compare!O20</f>
-        <v>657.56595386517267</v>
-      </c>
-      <c r="P20" s="16">
-        <f>1000000/Compare!P20</f>
-        <v>9523.8095238095229</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <f>'Teensy 3.2'!B15</f>
-        <v>256</v>
-      </c>
-      <c r="C21" s="16" t="e">
-        <f>1000000/Compare!C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" s="16" t="e">
-        <f>1000000/Compare!D21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="16">
-        <f>1000000/Compare!E21</f>
-        <v>3669.1861745064944</v>
-      </c>
-      <c r="F21" s="16">
-        <f>1000000/Compare!F21</f>
-        <v>7352.9411764705883</v>
-      </c>
-      <c r="H21" s="16" t="e">
-        <f>1000000/Compare!H21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" s="16" t="e">
-        <f>1000000/Compare!I21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" s="16">
-        <f>1000000/Compare!J21</f>
-        <v>1674.817444898506</v>
-      </c>
-      <c r="K21" s="16">
-        <f>1000000/Compare!K21</f>
-        <v>3154.5741324921137</v>
-      </c>
-      <c r="M21" s="16" t="e">
-        <f>1000000/Compare!M21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" s="16" t="e">
-        <f>1000000/Compare!N21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O21" s="16">
-        <f>1000000/Compare!O21</f>
-        <v>330.84975450948218</v>
-      </c>
-      <c r="P21" s="16">
-        <f>1000000/Compare!P21</f>
-        <v>4878.0487804878048</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <f>'Teensy 3.2'!B16</f>
-        <v>512</v>
-      </c>
-      <c r="C22" s="16" t="e">
-        <f>1000000/Compare!C22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D22" s="16" t="e">
-        <f>1000000/Compare!D22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" s="16">
-        <f>1000000/Compare!E22</f>
-        <v>1574.6543633672411</v>
-      </c>
-      <c r="F22" s="16">
-        <f>1000000/Compare!F22</f>
-        <v>3225.8064516129034</v>
-      </c>
-      <c r="H22" s="16" t="e">
-        <f>1000000/Compare!H22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" s="16" t="e">
-        <f>1000000/Compare!I22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" s="16">
-        <f>1000000/Compare!J22</f>
-        <v>677.43334055928892</v>
-      </c>
-      <c r="K22" s="16">
-        <f>1000000/Compare!K22</f>
-        <v>1272.2646310432569</v>
-      </c>
-      <c r="M22" s="16" t="e">
-        <f>1000000/Compare!M22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" s="16" t="e">
-        <f>1000000/Compare!N22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" s="16">
-        <f>1000000/Compare!O22</f>
-        <v>129.6798205231284</v>
-      </c>
-      <c r="P22" s="16">
-        <f>1000000/Compare!P22</f>
-        <v>2123.1422505307855</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <f>'Teensy 3.2'!B17</f>
-        <v>1024</v>
-      </c>
-      <c r="C23" s="16" t="e">
-        <f>1000000/Compare!C23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="16" t="e">
-        <f>1000000/Compare!D23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="16">
-        <f>1000000/Compare!E23</f>
-        <v>797.19387755102036</v>
-      </c>
-      <c r="F23" s="16">
-        <f>1000000/Compare!F23</f>
-        <v>1628.6644951140065</v>
-      </c>
-      <c r="H23" s="16" t="e">
-        <f>1000000/Compare!H23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" s="16" t="e">
-        <f>1000000/Compare!I23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" s="16">
-        <f>1000000/Compare!J23</f>
-        <v>342.43291739148299</v>
-      </c>
-      <c r="K23" s="16">
-        <f>1000000/Compare!K23</f>
-        <v>641.84852374839534</v>
-      </c>
-      <c r="M23" s="16" t="e">
-        <f>1000000/Compare!M23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" s="16" t="e">
-        <f>1000000/Compare!N23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O23" s="16">
-        <f>1000000/Compare!O23</f>
-        <v>65.006910234557935</v>
-      </c>
-      <c r="P23" s="16">
-        <f>1000000/Compare!P23</f>
-        <v>1077.5862068965516</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="3" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" customWidth="1"/>
-    <col min="8" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="3.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" t="str">
-        <f>'Arduino Uno'!$C$7</f>
-        <v>KissFFT</v>
-      </c>
-      <c r="H2" t="str">
-        <f>'Arduino Uno'!$C$7</f>
-        <v>KissFFT</v>
-      </c>
-      <c r="M2" t="str">
-        <f>'Arduino Uno'!$C$7</f>
-        <v>KissFFT</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C3" t="str">
-        <f>'Arduino Uno'!$C$6</f>
-        <v>Int16</v>
-      </c>
-      <c r="H3" t="str">
-        <f>'Arduino Uno'!$G$6</f>
-        <v>Int32</v>
-      </c>
-      <c r="M3" t="str">
-        <f>'Arduino Uno'!$K$6</f>
-        <v>Float</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" t="str">
-        <f>C4</f>
-        <v>usec per FFT</v>
-      </c>
-      <c r="M4" t="str">
-        <f>C4</f>
-        <v>usec per FFT</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="str">
-        <f>'Arduino Uno'!$C$2</f>
-        <v>Arduino Uno</v>
-      </c>
-      <c r="D5" t="str">
-        <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
-      </c>
-      <c r="E5" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="F5" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-      <c r="H5" t="str">
-        <f>'Arduino Uno'!$C$2</f>
-        <v>Arduino Uno</v>
-      </c>
-      <c r="I5" t="str">
-        <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
-      </c>
-      <c r="J5" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="K5" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-      <c r="M5" t="str">
-        <f>'Arduino Uno'!$C$2</f>
-        <v>Arduino Uno</v>
-      </c>
-      <c r="N5" t="str">
-        <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
-      </c>
-      <c r="O5" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="P5" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f>'Arduino Uno'!$B12</f>
-        <v>32</v>
-      </c>
-      <c r="C6" s="16">
-        <f>'Arduino Uno'!$C12</f>
-        <v>4980.8</v>
-      </c>
-      <c r="D6" s="16">
-        <f>'Arduino M0 Pro'!C12</f>
-        <v>319.8</v>
-      </c>
-      <c r="E6" s="16">
-        <f>'Teensy 3.2'!C12</f>
-        <v>103.4</v>
-      </c>
-      <c r="F6" s="16">
-        <f>'NXP K66'!C12</f>
-        <v>69</v>
-      </c>
-      <c r="H6" s="16">
-        <f>'Arduino Uno'!G12</f>
-        <v>12559.2</v>
-      </c>
-      <c r="I6" s="16">
-        <f>'Arduino M0 Pro'!G12</f>
-        <v>802</v>
-      </c>
-      <c r="J6" s="16">
-        <f>'Teensy 3.2'!G12</f>
-        <v>192.8</v>
-      </c>
-      <c r="K6" s="16">
-        <f>'NXP K66'!G12</f>
-        <v>102</v>
-      </c>
-      <c r="M6" s="16">
-        <f>'Arduino Uno'!K12</f>
-        <v>6378</v>
-      </c>
-      <c r="N6" s="16">
-        <f>'Arduino M0 Pro'!K12</f>
-        <v>2188</v>
-      </c>
-      <c r="O6" s="16">
-        <f>'Teensy 3.2'!K12</f>
-        <v>496.4</v>
-      </c>
-      <c r="P6" s="16">
-        <f>'NXP K66'!K12</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <f>'Arduino Uno'!$B13</f>
-        <v>64</v>
-      </c>
-      <c r="C7" s="16">
-        <f>'Arduino Uno'!$C13</f>
-        <v>10102.4</v>
-      </c>
-      <c r="D7" s="16">
-        <f>'Arduino M0 Pro'!C13</f>
-        <v>627.20000000000005</v>
-      </c>
-      <c r="E7" s="16">
-        <f>'Teensy 3.2'!C13</f>
-        <v>204.4</v>
-      </c>
-      <c r="F7" s="16">
-        <f>'NXP K66'!C13</f>
-        <v>136</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16">
-        <f>'Arduino M0 Pro'!G13</f>
-        <v>1674</v>
-      </c>
-      <c r="J7" s="16">
-        <f>'Teensy 3.2'!G13</f>
-        <v>383.6</v>
-      </c>
-      <c r="K7" s="16">
-        <f>'NXP K66'!G13</f>
-        <v>190</v>
-      </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16">
-        <f>'Arduino M0 Pro'!K13</f>
-        <v>5035</v>
-      </c>
-      <c r="O7" s="16">
-        <f>'Teensy 3.2'!K13</f>
-        <v>1136</v>
-      </c>
-      <c r="P7" s="16">
-        <f>'NXP K66'!K13</f>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <f>'Arduino Uno'!$B14</f>
-        <v>128</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16">
-        <f>'Arduino M0 Pro'!C14</f>
-        <v>1565</v>
-      </c>
-      <c r="E8" s="16">
-        <f>'Teensy 3.2'!C14</f>
-        <v>520.4</v>
-      </c>
-      <c r="F8" s="16">
-        <f>'NXP K66'!C14</f>
-        <v>349</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16">
-        <f>'Arduino M0 Pro'!G14</f>
-        <v>4241</v>
-      </c>
-      <c r="J8" s="16">
-        <f>'Teensy 3.2'!G14</f>
-        <v>993.2</v>
-      </c>
-      <c r="K8" s="16">
-        <f>'NXP K66'!G14</f>
-        <v>512</v>
-      </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16">
-        <f>'Arduino M0 Pro'!K14</f>
-        <v>12312</v>
-      </c>
-      <c r="O8" s="16">
-        <f>'Teensy 3.2'!K14</f>
-        <v>2849.8</v>
-      </c>
-      <c r="P8" s="16">
-        <f>'NXP K66'!K14</f>
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <f>'Arduino Uno'!$B15</f>
-        <v>256</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16">
-        <f>'Arduino M0 Pro'!C15</f>
-        <v>3079</v>
-      </c>
-      <c r="E9" s="16">
-        <f>'Teensy 3.2'!C15</f>
-        <v>1030.4000000000001</v>
-      </c>
-      <c r="F9" s="16">
-        <f>'NXP K66'!C15</f>
-        <v>686</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16">
-        <f>'Arduino M0 Pro'!G15</f>
-        <v>8763</v>
-      </c>
-      <c r="J9" s="16">
-        <f>'Teensy 3.2'!G15</f>
-        <v>1976</v>
-      </c>
-      <c r="K9" s="16">
-        <f>'NXP K66'!G15</f>
-        <v>970</v>
-      </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16">
-        <f>'Arduino M0 Pro'!K15</f>
-        <v>27349</v>
-      </c>
-      <c r="O9" s="16">
-        <f>'Teensy 3.2'!K15</f>
-        <v>6295.8</v>
-      </c>
-      <c r="P9" s="16">
-        <f>'NXP K66'!K15</f>
-        <v>371</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <f>'Arduino Uno'!$B16</f>
-        <v>512</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16">
-        <f>'Arduino M0 Pro'!C16</f>
-        <v>7403</v>
-      </c>
-      <c r="E10" s="16">
-        <f>'Teensy 3.2'!C16</f>
-        <v>2508</v>
-      </c>
-      <c r="F10" s="16">
-        <f>'NXP K66'!C16</f>
-        <v>1683</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16">
-        <f>'Arduino M0 Pro'!G16</f>
-        <v>21103</v>
-      </c>
-      <c r="J10" s="16">
-        <f>'Teensy 3.2'!G16</f>
-        <v>4858</v>
-      </c>
-      <c r="K10" s="16">
-        <f>'NXP K66'!G16</f>
-        <v>2461</v>
-      </c>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16">
-        <f>'Arduino M0 Pro'!K16</f>
-        <v>63732</v>
-      </c>
-      <c r="O10" s="16">
-        <f>'Teensy 3.2'!K16</f>
-        <v>14922</v>
-      </c>
-      <c r="P10" s="16">
-        <f>'NXP K66'!K16</f>
-        <v>981</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <f>'Arduino Uno'!$B17</f>
-        <v>1024</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16">
-        <f>'Arduino M0 Pro'!C17</f>
-        <v>14605.4</v>
-      </c>
-      <c r="E11" s="16">
-        <f>'Teensy 3.2'!C17</f>
-        <v>4975</v>
-      </c>
-      <c r="F11" s="16">
-        <f>'NXP K66'!C17</f>
-        <v>3316</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16">
-        <f>'Arduino M0 Pro'!G17</f>
-        <v>43329</v>
-      </c>
-      <c r="J11" s="16">
-        <f>'Teensy 3.2'!G17</f>
-        <v>9679</v>
-      </c>
-      <c r="K11" s="16">
-        <f>'NXP K66'!G17</f>
-        <v>4708</v>
-      </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16">
-        <f>'Arduino M0 Pro'!K17</f>
-        <v>138469</v>
-      </c>
-      <c r="O11" s="16">
-        <f>'Teensy 3.2'!K17</f>
-        <v>32259.4</v>
-      </c>
-      <c r="P11" s="16">
-        <f>'NXP K66'!K17</f>
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C14" t="str">
-        <f>'Teensy 3.2'!$E$7</f>
-        <v>CMSIS FFT</v>
-      </c>
-      <c r="E14" t="str">
-        <f>'Teensy 3.2'!E8</f>
-        <v>Radix4</v>
-      </c>
-      <c r="H14" t="str">
-        <f>'Teensy 3.2'!$E$7</f>
-        <v>CMSIS FFT</v>
-      </c>
-      <c r="M14" t="str">
-        <f>'Teensy 3.2'!$E$7</f>
-        <v>CMSIS FFT</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C15" t="str">
-        <f>'Arduino Uno'!$C$6</f>
-        <v>Int16</v>
-      </c>
-      <c r="H15" t="str">
-        <f>'Teensy 3.2'!$H$6</f>
-        <v>Int32</v>
-      </c>
-      <c r="M15" t="str">
-        <f>'Teensy 3.2'!$K$6</f>
-        <v>Float</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" t="str">
-        <f>C16</f>
-        <v>usec per FFT</v>
-      </c>
-      <c r="M16" t="str">
-        <f>C16</f>
-        <v>usec per FFT</v>
-      </c>
-      <c r="O16" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="P16" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="str">
-        <f>'Arduino Uno'!$C$2</f>
-        <v>Arduino Uno</v>
-      </c>
-      <c r="D17" t="str">
-        <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
-      </c>
-      <c r="E17" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="F17" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-      <c r="H17" t="str">
-        <f>'Arduino Uno'!$C$2</f>
-        <v>Arduino Uno</v>
-      </c>
-      <c r="I17" t="str">
-        <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
-      </c>
-      <c r="J17" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="K17" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
-      </c>
-      <c r="M17" t="str">
-        <f>'Arduino Uno'!$C$2</f>
-        <v>Arduino Uno</v>
-      </c>
-      <c r="N17" t="str">
-        <f>'Arduino M0 Pro'!$C$2</f>
-        <v>Arduino M0 Pro</v>
-      </c>
-      <c r="O17" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="P17" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>NXP K66</v>
+        <v>FRDM-K66F</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -12673,14 +13519,14 @@
   <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:K17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Benchmark: Update FFT analysis for blog
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="14" r:id="rId1"/>
-    <sheet name="Summary Table" sheetId="13" r:id="rId2"/>
+    <sheet name="Summary For Blog" sheetId="13" r:id="rId2"/>
     <sheet name="Summary_Speed" sheetId="9" r:id="rId3"/>
     <sheet name="Summary-Duration" sheetId="6" r:id="rId4"/>
     <sheet name="AllData" sheetId="7" r:id="rId5"/>
@@ -590,7 +590,29 @@
     <xf numFmtId="37" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -599,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -617,34 +639,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -711,7 +711,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1600"/>
-              <a:t>FFTs Per Second</a:t>
+              <a:t>FFTs Per Second, Int32</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -739,7 +739,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$L$13</c:f>
+              <c:f>'Summary For Blog'!$L$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -750,7 +750,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -774,7 +774,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$L$14:$L$18</c:f>
+              <c:f>'Summary For Blog'!$L$14:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -803,7 +803,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$M$13</c:f>
+              <c:f>'Summary For Blog'!$M$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -814,7 +814,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -838,7 +838,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$M$14:$M$18</c:f>
+              <c:f>'Summary For Blog'!$M$14:$M$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -867,7 +867,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$N$13</c:f>
+              <c:f>'Summary For Blog'!$N$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -878,7 +878,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -902,7 +902,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$N$14:$N$18</c:f>
+              <c:f>'Summary For Blog'!$N$14:$N$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -931,7 +931,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$O$13</c:f>
+              <c:f>'Summary For Blog'!$O$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -942,7 +942,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -966,7 +966,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$O$14:$O$18</c:f>
+              <c:f>'Summary For Blog'!$O$14:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -995,7 +995,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$P$13</c:f>
+              <c:f>'Summary For Blog'!$P$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1006,7 +1006,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1030,7 +1030,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$P$14:$P$18</c:f>
+              <c:f>'Summary For Blog'!$P$14:$P$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1059,7 +1059,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$R$13</c:f>
+              <c:f>'Summary For Blog'!$R$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1070,7 +1070,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1094,7 +1094,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$R$14:$R$18</c:f>
+              <c:f>'Summary For Blog'!$R$14:$R$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1123,7 +1123,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$S$13</c:f>
+              <c:f>'Summary For Blog'!$S$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1134,7 +1134,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'Summary Table'!$B$14:$B$18</c:f>
+              <c:f>'Summary For Blog'!$B$14:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1158,7 +1158,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$S$14:$S$18</c:f>
+              <c:f>'Summary For Blog'!$S$14:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1192,11 +1192,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145706368"/>
-        <c:axId val="145712256"/>
+        <c:axId val="154062848"/>
+        <c:axId val="154064768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145706368"/>
+        <c:axId val="154062848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,7 +1225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145712256"/>
+        <c:crossAx val="154064768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1233,7 +1233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145712256"/>
+        <c:axId val="154064768"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1265,7 +1265,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145706368"/>
+        <c:crossAx val="154062848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1492,11 +1492,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144942592"/>
-        <c:axId val="144944128"/>
+        <c:axId val="159099904"/>
+        <c:axId val="159101696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144942592"/>
+        <c:axId val="159099904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1505,7 +1505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144944128"/>
+        <c:crossAx val="159101696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1513,7 +1513,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144944128"/>
+        <c:axId val="159101696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144942592"/>
+        <c:crossAx val="159099904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1950,11 +1950,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146351232"/>
-        <c:axId val="146352768"/>
+        <c:axId val="159394432"/>
+        <c:axId val="159420800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146351232"/>
+        <c:axId val="159394432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,7 +1963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146352768"/>
+        <c:crossAx val="159420800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1971,7 +1971,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146352768"/>
+        <c:axId val="159420800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,7 +2000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146351232"/>
+        <c:crossAx val="159394432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -2335,11 +2335,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145877248"/>
-        <c:axId val="146145664"/>
+        <c:axId val="159219712"/>
+        <c:axId val="159221632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145877248"/>
+        <c:axId val="159219712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,7 +2367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146145664"/>
+        <c:crossAx val="159221632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2375,7 +2375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146145664"/>
+        <c:axId val="159221632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2407,7 +2407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145877248"/>
+        <c:crossAx val="159219712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2741,11 +2741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146181120"/>
-        <c:axId val="146187392"/>
+        <c:axId val="159257344"/>
+        <c:axId val="159259264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146181120"/>
+        <c:axId val="159257344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146187392"/>
+        <c:crossAx val="159259264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2781,7 +2781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146187392"/>
+        <c:axId val="159259264"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2813,7 +2813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146181120"/>
+        <c:crossAx val="159257344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3092,11 +3092,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146283520"/>
-        <c:axId val="146293888"/>
+        <c:axId val="159281920"/>
+        <c:axId val="159283840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146283520"/>
+        <c:axId val="159281920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3124,7 +3124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146293888"/>
+        <c:crossAx val="159283840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3132,7 +3132,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146293888"/>
+        <c:axId val="159283840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3161,7 +3161,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146283520"/>
+        <c:crossAx val="159281920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3440,11 +3440,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146308480"/>
-        <c:axId val="146331136"/>
+        <c:axId val="159794304"/>
+        <c:axId val="159796224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146308480"/>
+        <c:axId val="159794304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3472,7 +3472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146331136"/>
+        <c:crossAx val="159796224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3480,7 +3480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146331136"/>
+        <c:axId val="159796224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3509,7 +3509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146308480"/>
+        <c:crossAx val="159794304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3788,11 +3788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146705408"/>
-        <c:axId val="146707584"/>
+        <c:axId val="159515392"/>
+        <c:axId val="159517312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146705408"/>
+        <c:axId val="159515392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,7 +3820,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146707584"/>
+        <c:crossAx val="159517312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3828,7 +3828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146707584"/>
+        <c:axId val="159517312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3857,7 +3857,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146705408"/>
+        <c:crossAx val="159515392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4118,11 +4118,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146545664"/>
-        <c:axId val="146547840"/>
+        <c:axId val="159548160"/>
+        <c:axId val="159550080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146545664"/>
+        <c:axId val="159548160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4150,7 +4150,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146547840"/>
+        <c:crossAx val="159550080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4158,7 +4158,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146547840"/>
+        <c:axId val="159550080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4187,7 +4187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146545664"/>
+        <c:crossAx val="159548160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4448,11 +4448,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146586624"/>
-        <c:axId val="146592896"/>
+        <c:axId val="159585024"/>
+        <c:axId val="159586944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146586624"/>
+        <c:axId val="159585024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4480,7 +4480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146592896"/>
+        <c:crossAx val="159586944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4488,7 +4488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146592896"/>
+        <c:axId val="159586944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4517,7 +4517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146586624"/>
+        <c:crossAx val="159585024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4778,11 +4778,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146488704"/>
-        <c:axId val="146511360"/>
+        <c:axId val="159630464"/>
+        <c:axId val="159632384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146488704"/>
+        <c:axId val="159630464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4810,7 +4810,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146511360"/>
+        <c:crossAx val="159632384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4818,7 +4818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146511360"/>
+        <c:axId val="159632384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4847,7 +4847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146488704"/>
+        <c:crossAx val="159630464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4932,7 +4932,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$C$16</c:f>
+              <c:f>'Summary For Blog'!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4944,7 +4944,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Summary Table'!$M$13:$P$13</c:f>
+              <c:f>'Summary For Blog'!$M$13:$P$13</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -4964,7 +4964,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$M$16:$P$16</c:f>
+              <c:f>'Summary For Blog'!$M$16:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4993,11 +4993,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145740544"/>
-        <c:axId val="145742080"/>
+        <c:axId val="157956352"/>
+        <c:axId val="157966336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145740544"/>
+        <c:axId val="157956352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5006,7 +5006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145742080"/>
+        <c:crossAx val="157966336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5014,7 +5014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145742080"/>
+        <c:axId val="157966336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5025,7 +5025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145740544"/>
+        <c:crossAx val="157956352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5111,7 +5111,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$C$16</c:f>
+              <c:f>'Summary For Blog'!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5123,7 +5123,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Summary Table'!$M$13:$P$13</c:f>
+              <c:f>'Summary For Blog'!$M$13:$P$13</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5143,7 +5143,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$M$16:$P$16</c:f>
+              <c:f>'Summary For Blog'!$M$16:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5168,7 +5168,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$C$25</c:f>
+              <c:f>'Summary For Blog'!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5180,7 +5180,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Summary Table'!$M$13:$P$13</c:f>
+              <c:f>'Summary For Blog'!$M$13:$P$13</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5200,7 +5200,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$M$25:$P$25</c:f>
+              <c:f>'Summary For Blog'!$M$25:$P$25</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5229,11 +5229,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145642240"/>
-        <c:axId val="145643776"/>
+        <c:axId val="157989120"/>
+        <c:axId val="157990912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145642240"/>
+        <c:axId val="157989120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5242,7 +5242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145643776"/>
+        <c:crossAx val="157990912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5250,7 +5250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145643776"/>
+        <c:axId val="157990912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5261,7 +5261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145642240"/>
+        <c:crossAx val="157989120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -5333,7 +5333,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5348,7 +5347,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$C$16</c:f>
+              <c:f>'Summary For Blog'!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5360,7 +5359,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Summary Table'!$M$13:$S$13</c:f>
+              <c:f>'Summary For Blog'!$M$13:$S$13</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5386,7 +5385,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$M$16:$S$16</c:f>
+              <c:f>'Summary For Blog'!$M$16:$S$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5417,7 +5416,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Summary Table'!$C$25</c:f>
+              <c:f>'Summary For Blog'!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5429,7 +5428,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Summary Table'!$M$13:$S$13</c:f>
+              <c:f>'Summary For Blog'!$M$13:$S$13</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -5455,7 +5454,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Summary Table'!$M$25:$S$25</c:f>
+              <c:f>'Summary For Blog'!$M$25:$S$25</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="7"/>
@@ -5490,11 +5489,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145652736"/>
-        <c:axId val="145679104"/>
+        <c:axId val="157998080"/>
+        <c:axId val="158028544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145652736"/>
+        <c:axId val="157998080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5503,7 +5502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145679104"/>
+        <c:crossAx val="158028544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5511,7 +5510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145679104"/>
+        <c:axId val="158028544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5522,7 +5521,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145652736"/>
+        <c:crossAx val="157998080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -5530,7 +5529,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5874,11 +5872,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144856576"/>
-        <c:axId val="144858496"/>
+        <c:axId val="153871488"/>
+        <c:axId val="153873408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144856576"/>
+        <c:axId val="153871488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5906,7 +5904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144858496"/>
+        <c:crossAx val="153873408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5914,7 +5912,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144858496"/>
+        <c:axId val="153873408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5945,7 +5943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144856576"/>
+        <c:crossAx val="153871488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6302,11 +6300,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145781504"/>
-        <c:axId val="145783424"/>
+        <c:axId val="153909504"/>
+        <c:axId val="153911680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145781504"/>
+        <c:axId val="153909504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6334,7 +6332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145783424"/>
+        <c:crossAx val="153911680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6342,7 +6340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145783424"/>
+        <c:axId val="153911680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6373,7 +6371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145781504"/>
+        <c:crossAx val="153909504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6545,11 +6543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144776576"/>
-        <c:axId val="144778368"/>
+        <c:axId val="158610176"/>
+        <c:axId val="158611712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144776576"/>
+        <c:axId val="158610176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6558,7 +6556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144778368"/>
+        <c:crossAx val="158611712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6566,7 +6564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144778368"/>
+        <c:axId val="158611712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -6596,7 +6594,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144776576"/>
+        <c:crossAx val="158610176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -6723,11 +6721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="144807424"/>
-        <c:axId val="144808960"/>
+        <c:axId val="158628480"/>
+        <c:axId val="158646656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="144807424"/>
+        <c:axId val="158628480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6738,12 +6736,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144808960"/>
+        <c:crossAx val="158646656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144808960"/>
+        <c:axId val="158646656"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6755,7 +6753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144807424"/>
+        <c:crossAx val="158628480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6996,11 +6994,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144910976"/>
-        <c:axId val="144916864"/>
+        <c:axId val="159064448"/>
+        <c:axId val="159065984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144910976"/>
+        <c:axId val="159064448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7009,7 +7007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144916864"/>
+        <c:crossAx val="159065984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7017,7 +7015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144916864"/>
+        <c:axId val="159065984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -7055,7 +7053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144910976"/>
+        <c:crossAx val="159064448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8135,7 +8133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -8153,191 +8151,191 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="29" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="30" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="30" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="44" t="s">
+      <c r="I9" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="30" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="30" t="s">
         <v>107</v>
       </c>
     </row>
@@ -8745,8 +8743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8760,34 +8758,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="27"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="str">
@@ -9179,45 +9177,45 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="26" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="str">
@@ -9608,48 +9606,48 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="str">
+      <c r="B21" s="35" t="str">
         <f t="shared" ref="B21:B27" si="14">B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="26" t="str">
+      <c r="C21" s="35"/>
+      <c r="D21" s="36" t="str">
         <f>D12</f>
         <v>Generic C</v>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27" t="str">
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37" t="str">
         <f>I12</f>
         <v>CMSIS</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="37"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="str">
@@ -10041,17 +10039,17 @@
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -10096,42 +10094,42 @@
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29" t="s">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="31"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="41"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="32" t="str">
+      <c r="B32" s="42" t="str">
         <f>B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="26" t="str">
+      <c r="C32" s="43"/>
+      <c r="D32" s="36" t="str">
         <f>D12</f>
         <v>Generic C</v>
       </c>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27" t="str">
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37" t="str">
         <f>I12</f>
         <v>CMSIS</v>
       </c>
-      <c r="J32" s="27"/>
-      <c r="Q32" s="28" t="s">
+      <c r="J32" s="37"/>
+      <c r="Q32" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="R32" s="28"/>
-      <c r="S32" s="28"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="str">
@@ -10176,14 +10174,14 @@
       <c r="M33" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q33" s="37" t="s">
+      <c r="Q33" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="R33" s="37" t="str">
+      <c r="R33" s="25" t="str">
         <f>I33</f>
         <v>Teensy 3.2</v>
       </c>
-      <c r="S33" s="37" t="str">
+      <c r="S33" s="25" t="str">
         <f>J33</f>
         <v>FRDM-K66F</v>
       </c>
@@ -10231,15 +10229,15 @@
         <f>1/(1-M33)</f>
         <v>2</v>
       </c>
-      <c r="Q34" s="38" t="str">
+      <c r="Q34" s="26" t="str">
         <f>C34</f>
         <v>Int16</v>
       </c>
-      <c r="R34" s="39">
+      <c r="R34" s="27">
         <f>I7/G7</f>
         <v>3.724058966652354</v>
       </c>
-      <c r="S34" s="39">
+      <c r="S34" s="27">
         <f>J7/H7</f>
         <v>4.9857142857142867</v>
       </c>
@@ -10287,15 +10285,15 @@
         <f>M34</f>
         <v>2</v>
       </c>
-      <c r="Q35" s="38" t="str">
+      <c r="Q35" s="26" t="str">
         <f>C35</f>
         <v>Int32</v>
       </c>
-      <c r="R35" s="39">
+      <c r="R35" s="27">
         <f>I16/G16</f>
         <v>3.2703325650312816</v>
       </c>
-      <c r="S35" s="39">
+      <c r="S35" s="27">
         <f>J16/H16</f>
         <v>3.1801242236024843</v>
       </c>
@@ -10343,34 +10341,43 @@
         <f>M34+M35</f>
         <v>4</v>
       </c>
-      <c r="Q36" s="38" t="str">
+      <c r="Q36" s="26" t="str">
         <f>C36</f>
         <v>Float32</v>
       </c>
-      <c r="R36" s="39">
+      <c r="R36" s="27">
         <f>I25/G25</f>
         <v>1.8739314553249691</v>
       </c>
-      <c r="S36" s="39">
+      <c r="S36" s="27">
         <f>J25/H25</f>
         <v>2.0666666666666664</v>
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B28:J28"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
@@ -10383,19 +10390,10 @@
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="D32:H32"/>
     <mergeCell ref="I32:J32"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B28:J28"/>
     <mergeCell ref="B19:J19"/>
     <mergeCell ref="D11:J11"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D12:H12"/>
-    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:J36">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -10430,39 +10428,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="W2" s="36" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="W2" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
     </row>
     <row r="4" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C4" t="str">
@@ -12162,46 +12160,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:41" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="X2" s="36" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="X2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="36"/>
-      <c r="AJ2" s="36"/>
-      <c r="AK2" s="36"/>
-      <c r="AL2" s="36"/>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="36"/>
-      <c r="AO2" s="36"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="45"/>
+      <c r="AC2" s="45"/>
+      <c r="AD2" s="45"/>
+      <c r="AE2" s="45"/>
+      <c r="AF2" s="45"/>
+      <c r="AG2" s="45"/>
+      <c r="AH2" s="45"/>
+      <c r="AI2" s="45"/>
+      <c r="AJ2" s="45"/>
+      <c r="AK2" s="45"/>
+      <c r="AL2" s="45"/>
+      <c r="AM2" s="45"/>
+      <c r="AN2" s="45"/>
+      <c r="AO2" s="45"/>
     </row>
     <row r="4" spans="2:41" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="str">

</xml_diff>

<commit_message>
Benchmark: tweak FFT XLS for blog
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="14" r:id="rId1"/>
@@ -402,7 +402,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,8 +467,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -660,10 +674,10 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,6 +710,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -892,11 +910,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="86652800"/>
-        <c:axId val="86654336"/>
+        <c:axId val="43614592"/>
+        <c:axId val="43616128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86652800"/>
+        <c:axId val="43614592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86654336"/>
+        <c:crossAx val="43616128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -913,7 +931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86654336"/>
+        <c:axId val="43616128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,7 +942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86652800"/>
+        <c:crossAx val="43614592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1051,11 +1069,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145891328"/>
-        <c:axId val="145892864"/>
+        <c:axId val="44905216"/>
+        <c:axId val="44906752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145891328"/>
+        <c:axId val="44905216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1066,12 +1084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145892864"/>
+        <c:crossAx val="44906752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145892864"/>
+        <c:axId val="44906752"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1083,7 +1101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145891328"/>
+        <c:crossAx val="44905216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1360,11 +1378,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145920384"/>
-        <c:axId val="145921920"/>
+        <c:axId val="44931712"/>
+        <c:axId val="44949888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145920384"/>
+        <c:axId val="44931712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145921920"/>
+        <c:crossAx val="44949888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1381,7 +1399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145921920"/>
+        <c:axId val="44949888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -1419,7 +1437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145920384"/>
+        <c:crossAx val="44931712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,11 +1666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146221696"/>
-        <c:axId val="146227584"/>
+        <c:axId val="44983808"/>
+        <c:axId val="44985344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146221696"/>
+        <c:axId val="44983808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,7 +1679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146227584"/>
+        <c:crossAx val="44985344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1669,7 +1687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146227584"/>
+        <c:axId val="44985344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +1733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146221696"/>
+        <c:crossAx val="44983808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1780,7 +1798,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2170,11 +2187,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="146258176"/>
-        <c:axId val="146087936"/>
+        <c:axId val="45020288"/>
+        <c:axId val="45021824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146258176"/>
+        <c:axId val="45020288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2183,7 +2200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146087936"/>
+        <c:crossAx val="45021824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2191,7 +2208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146087936"/>
+        <c:axId val="45021824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2214,14 +2231,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146258176"/>
+        <c:crossAx val="45020288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -2229,7 +2245,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2627,11 +2642,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145637376"/>
-        <c:axId val="145639296"/>
+        <c:axId val="44223104"/>
+        <c:axId val="44229376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145637376"/>
+        <c:axId val="44223104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,7 +2674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145639296"/>
+        <c:crossAx val="44229376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2667,7 +2682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145639296"/>
+        <c:axId val="44229376"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2699,7 +2714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145637376"/>
+        <c:crossAx val="44223104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3103,11 +3118,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146105856"/>
-        <c:axId val="146107776"/>
+        <c:axId val="44306816"/>
+        <c:axId val="44308736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146105856"/>
+        <c:axId val="44306816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3150,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146107776"/>
+        <c:crossAx val="44308736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3143,7 +3158,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146107776"/>
+        <c:axId val="44308736"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3175,7 +3190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146105856"/>
+        <c:crossAx val="44306816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3454,11 +3469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145720832"/>
-        <c:axId val="145722752"/>
+        <c:axId val="44351872"/>
+        <c:axId val="44353792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145720832"/>
+        <c:axId val="44351872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3486,7 +3501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145722752"/>
+        <c:crossAx val="44353792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3494,7 +3509,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145722752"/>
+        <c:axId val="44353792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3523,7 +3538,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145720832"/>
+        <c:crossAx val="44351872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3802,11 +3817,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145774080"/>
-        <c:axId val="145776000"/>
+        <c:axId val="44843392"/>
+        <c:axId val="44845312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145774080"/>
+        <c:axId val="44843392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,7 +3849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145776000"/>
+        <c:crossAx val="44845312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3842,7 +3857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145776000"/>
+        <c:axId val="44845312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3871,7 +3886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145774080"/>
+        <c:crossAx val="44843392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4150,11 +4165,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145810944"/>
-        <c:axId val="145812864"/>
+        <c:axId val="44884352"/>
+        <c:axId val="44886272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145810944"/>
+        <c:axId val="44884352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4182,7 +4197,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145812864"/>
+        <c:crossAx val="44886272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4190,7 +4205,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145812864"/>
+        <c:axId val="44886272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4219,7 +4234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145810944"/>
+        <c:crossAx val="44884352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4480,11 +4495,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146576896"/>
-        <c:axId val="146578816"/>
+        <c:axId val="98865536"/>
+        <c:axId val="98867456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146576896"/>
+        <c:axId val="98865536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4512,7 +4527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146578816"/>
+        <c:crossAx val="98867456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4520,7 +4535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146578816"/>
+        <c:axId val="98867456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4549,7 +4564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146576896"/>
+        <c:crossAx val="98865536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4776,11 +4791,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="88961792"/>
-        <c:axId val="88963328"/>
+        <c:axId val="43977344"/>
+        <c:axId val="43979136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88961792"/>
+        <c:axId val="43977344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4789,7 +4804,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88963328"/>
+        <c:crossAx val="43979136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4797,7 +4812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88963328"/>
+        <c:axId val="43979136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4808,7 +4823,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88961792"/>
+        <c:crossAx val="43977344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5070,11 +5085,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147006976"/>
-        <c:axId val="147008896"/>
+        <c:axId val="143139200"/>
+        <c:axId val="143141120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147006976"/>
+        <c:axId val="143139200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5102,7 +5117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147008896"/>
+        <c:crossAx val="143141120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5110,7 +5125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147008896"/>
+        <c:axId val="143141120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5139,7 +5154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147006976"/>
+        <c:crossAx val="143139200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5400,11 +5415,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147048320"/>
-        <c:axId val="147054592"/>
+        <c:axId val="143180544"/>
+        <c:axId val="143182464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147048320"/>
+        <c:axId val="143180544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5432,7 +5447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147054592"/>
+        <c:crossAx val="143182464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5440,7 +5455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147054592"/>
+        <c:axId val="143182464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5469,7 +5484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147048320"/>
+        <c:crossAx val="143180544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5529,7 +5544,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5996,11 +6010,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145574528"/>
-        <c:axId val="145584896"/>
+        <c:axId val="43801600"/>
+        <c:axId val="43807872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145574528"/>
+        <c:axId val="43801600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6022,14 +6036,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145584896"/>
+        <c:crossAx val="43807872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6037,7 +6050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145584896"/>
+        <c:axId val="43807872"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6062,14 +6075,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145574528"/>
+        <c:crossAx val="43801600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6149,7 +6161,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6237,11 +6248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145602048"/>
-        <c:axId val="145603584"/>
+        <c:axId val="44025728"/>
+        <c:axId val="44027264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145602048"/>
+        <c:axId val="44025728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6250,7 +6261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145603584"/>
+        <c:crossAx val="44027264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6258,7 +6269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145603584"/>
+        <c:axId val="44027264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6269,14 +6280,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145602048"/>
+        <c:crossAx val="44025728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6340,7 +6350,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6497,11 +6506,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145313792"/>
-        <c:axId val="145315328"/>
+        <c:axId val="43729664"/>
+        <c:axId val="43731200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145313792"/>
+        <c:axId val="43729664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6510,7 +6519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145315328"/>
+        <c:crossAx val="43731200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6518,7 +6527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145315328"/>
+        <c:axId val="43731200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6529,14 +6538,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145313792"/>
+        <c:crossAx val="43729664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6600,7 +6608,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6805,11 +6812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145344768"/>
-        <c:axId val="145350656"/>
+        <c:axId val="43759104"/>
+        <c:axId val="43760640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145344768"/>
+        <c:axId val="43759104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6818,7 +6825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145350656"/>
+        <c:crossAx val="43760640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6826,7 +6833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145350656"/>
+        <c:axId val="43760640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6837,14 +6844,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145344768"/>
+        <c:crossAx val="43759104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6890,7 +6896,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7189,11 +7194,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144783616"/>
-        <c:axId val="144785792"/>
+        <c:axId val="44068224"/>
+        <c:axId val="44078592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144783616"/>
+        <c:axId val="44068224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7215,14 +7220,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144785792"/>
+        <c:crossAx val="44078592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7230,7 +7234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144785792"/>
+        <c:axId val="44078592"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7255,21 +7259,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144783616"/>
+        <c:crossAx val="44068224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7322,7 +7324,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7621,11 +7622,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144821632"/>
-        <c:axId val="145491456"/>
+        <c:axId val="44536192"/>
+        <c:axId val="44538112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144821632"/>
+        <c:axId val="44536192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7647,14 +7648,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145491456"/>
+        <c:crossAx val="44538112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7662,7 +7662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145491456"/>
+        <c:axId val="44538112"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7687,21 +7687,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144821632"/>
+        <c:crossAx val="44536192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7760,7 +7758,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7892,11 +7889,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="145512704"/>
-        <c:axId val="145514496"/>
+        <c:axId val="44550784"/>
+        <c:axId val="44552576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145512704"/>
+        <c:axId val="44550784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7905,7 +7902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145514496"/>
+        <c:crossAx val="44552576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7913,7 +7910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145514496"/>
+        <c:axId val="44552576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -7937,14 +7934,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145512704"/>
+        <c:crossAx val="44550784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -7952,7 +7948,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9095,8 +9090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="B4:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9302,60 +9297,60 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="49" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="49" t="s">
         <v>107</v>
       </c>
     </row>
@@ -11041,7 +11036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B31" sqref="B31:I37"/>
     </sheetView>
   </sheetViews>
@@ -11054,16 +11049,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
@@ -11317,26 +11312,26 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="46" t="s">
@@ -11591,26 +11586,26 @@
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="46" t="str">
@@ -11867,16 +11862,16 @@
       <c r="Q27" s="10"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -11916,8 +11911,8 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="39" t="s">
         <v>70</v>
       </c>
@@ -12107,30 +12102,25 @@
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:I3"/>
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
@@ -12138,12 +12128,17 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:I32"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:I36">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
@@ -12177,21 +12172,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
@@ -12794,36 +12789,36 @@
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="46" t="s">
@@ -13429,36 +13424,36 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="46" t="str">
@@ -14068,21 +14063,21 @@
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -14147,8 +14142,8 @@
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="39" t="s">
         <v>70</v>
       </c>
@@ -14186,13 +14181,13 @@
       <c r="L32" s="45"/>
       <c r="M32" s="45"/>
       <c r="N32" s="45"/>
-      <c r="W32" s="37" t="s">
+      <c r="W32" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="X32" s="37"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="37"/>
-      <c r="AA32" s="37"/>
+      <c r="X32" s="38"/>
+      <c r="Y32" s="38"/>
+      <c r="Z32" s="38"/>
+      <c r="AA32" s="38"/>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="str">
@@ -14514,24 +14509,33 @@
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:N31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B28:N28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="W32:AA32"/>
@@ -14548,15 +14552,6 @@
     <mergeCell ref="D20:N20"/>
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="K12:N12"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:N31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B28:N28"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:N36">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Benchmark: update FFT XLS with Teensy rel speeds
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="19155" windowHeight="9015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="14" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="124">
   <si>
     <t>N</t>
   </si>
@@ -393,6 +393,15 @@
   <si>
     <t>Generic C FFT</t>
   </si>
+  <si>
+    <t>Clock Speed</t>
+  </si>
+  <si>
+    <t>Speed Relative to Teensy 3.2 (128-pt CMSIS FFT)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
@@ -402,7 +411,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +479,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -600,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -668,6 +685,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -678,6 +699,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -695,25 +725,24 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -910,11 +939,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43614592"/>
-        <c:axId val="43616128"/>
+        <c:axId val="147113088"/>
+        <c:axId val="147114624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43614592"/>
+        <c:axId val="147113088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43616128"/>
+        <c:crossAx val="147114624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -931,7 +960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43616128"/>
+        <c:axId val="147114624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43614592"/>
+        <c:crossAx val="147113088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1069,11 +1098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="44905216"/>
-        <c:axId val="44906752"/>
+        <c:axId val="148399616"/>
+        <c:axId val="148401152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44905216"/>
+        <c:axId val="148399616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1084,12 +1113,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44906752"/>
+        <c:crossAx val="148401152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44906752"/>
+        <c:axId val="148401152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1101,7 +1130,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44905216"/>
+        <c:crossAx val="148399616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1378,11 +1407,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44931712"/>
-        <c:axId val="44949888"/>
+        <c:axId val="148422016"/>
+        <c:axId val="148444288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44931712"/>
+        <c:axId val="148422016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,7 +1420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44949888"/>
+        <c:crossAx val="148444288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1399,7 +1428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44949888"/>
+        <c:axId val="148444288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -1437,7 +1466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44931712"/>
+        <c:crossAx val="148422016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1666,11 +1695,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44983808"/>
-        <c:axId val="44985344"/>
+        <c:axId val="148482304"/>
+        <c:axId val="148488192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44983808"/>
+        <c:axId val="148482304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1679,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44985344"/>
+        <c:crossAx val="148488192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1687,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44985344"/>
+        <c:axId val="148488192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1733,7 +1762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44983808"/>
+        <c:crossAx val="148482304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,11 +2216,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45020288"/>
-        <c:axId val="45021824"/>
+        <c:axId val="148248448"/>
+        <c:axId val="148249984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45020288"/>
+        <c:axId val="148248448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45021824"/>
+        <c:crossAx val="148249984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2208,7 +2237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45021824"/>
+        <c:axId val="148249984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2237,7 +2266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45020288"/>
+        <c:crossAx val="148248448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -2642,11 +2671,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44223104"/>
-        <c:axId val="44229376"/>
+        <c:axId val="147910016"/>
+        <c:axId val="147789312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44223104"/>
+        <c:axId val="147910016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2674,7 +2703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44229376"/>
+        <c:crossAx val="147789312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2682,7 +2711,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44229376"/>
+        <c:axId val="147789312"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2714,7 +2743,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44223104"/>
+        <c:crossAx val="147910016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3118,11 +3147,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44306816"/>
-        <c:axId val="44308736"/>
+        <c:axId val="147821696"/>
+        <c:axId val="147823616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44306816"/>
+        <c:axId val="147821696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3150,7 +3179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44308736"/>
+        <c:crossAx val="147823616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3158,7 +3187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44308736"/>
+        <c:axId val="147823616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3190,7 +3219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44306816"/>
+        <c:crossAx val="147821696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3469,11 +3498,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44351872"/>
-        <c:axId val="44353792"/>
+        <c:axId val="148296832"/>
+        <c:axId val="148298752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44351872"/>
+        <c:axId val="148296832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3501,7 +3530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44353792"/>
+        <c:crossAx val="148298752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3509,7 +3538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44353792"/>
+        <c:axId val="148298752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3538,7 +3567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44351872"/>
+        <c:crossAx val="148296832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3817,11 +3846,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44843392"/>
-        <c:axId val="44845312"/>
+        <c:axId val="148014208"/>
+        <c:axId val="148016128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44843392"/>
+        <c:axId val="148014208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3849,7 +3878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44845312"/>
+        <c:crossAx val="148016128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3857,7 +3886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44845312"/>
+        <c:axId val="148016128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3886,7 +3915,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44843392"/>
+        <c:crossAx val="148014208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4165,11 +4194,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44884352"/>
-        <c:axId val="44886272"/>
+        <c:axId val="148771968"/>
+        <c:axId val="148773888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44884352"/>
+        <c:axId val="148771968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4197,7 +4226,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44886272"/>
+        <c:crossAx val="148773888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4205,7 +4234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44886272"/>
+        <c:axId val="148773888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4234,7 +4263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44884352"/>
+        <c:crossAx val="148771968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4495,11 +4524,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98865536"/>
-        <c:axId val="98867456"/>
+        <c:axId val="148817024"/>
+        <c:axId val="148818944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98865536"/>
+        <c:axId val="148817024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4527,7 +4556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98867456"/>
+        <c:crossAx val="148818944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4535,7 +4564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98867456"/>
+        <c:axId val="148818944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4564,7 +4593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98865536"/>
+        <c:crossAx val="148817024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4791,11 +4820,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43977344"/>
-        <c:axId val="43979136"/>
+        <c:axId val="147479936"/>
+        <c:axId val="147481728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43977344"/>
+        <c:axId val="147479936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4804,7 +4833,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43979136"/>
+        <c:crossAx val="147481728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4812,7 +4841,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43979136"/>
+        <c:axId val="147481728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4823,7 +4852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43977344"/>
+        <c:crossAx val="147479936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5085,11 +5114,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143139200"/>
-        <c:axId val="143141120"/>
+        <c:axId val="148845696"/>
+        <c:axId val="148847616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143139200"/>
+        <c:axId val="148845696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5117,7 +5146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143141120"/>
+        <c:crossAx val="148847616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5125,7 +5154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143141120"/>
+        <c:axId val="148847616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5154,7 +5183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143139200"/>
+        <c:crossAx val="148845696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5415,11 +5444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143180544"/>
-        <c:axId val="143182464"/>
+        <c:axId val="153429504"/>
+        <c:axId val="153431424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143180544"/>
+        <c:axId val="153429504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5447,7 +5476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143182464"/>
+        <c:crossAx val="153431424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5455,7 +5484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143182464"/>
+        <c:axId val="153431424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5484,7 +5513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143180544"/>
+        <c:crossAx val="153429504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6010,11 +6039,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43801600"/>
-        <c:axId val="43807872"/>
+        <c:axId val="147646720"/>
+        <c:axId val="147521920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43801600"/>
+        <c:axId val="147646720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6042,7 +6071,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43807872"/>
+        <c:crossAx val="147521920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6050,7 +6079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43807872"/>
+        <c:axId val="147521920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6081,7 +6110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43801600"/>
+        <c:crossAx val="147646720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6248,11 +6277,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44025728"/>
-        <c:axId val="44027264"/>
+        <c:axId val="144329344"/>
+        <c:axId val="146694528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44025728"/>
+        <c:axId val="144329344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6261,7 +6290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44027264"/>
+        <c:crossAx val="146694528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6269,7 +6298,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44027264"/>
+        <c:axId val="146694528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6280,7 +6309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44025728"/>
+        <c:crossAx val="144329344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6506,11 +6535,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43729664"/>
-        <c:axId val="43731200"/>
+        <c:axId val="147559552"/>
+        <c:axId val="147561088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43729664"/>
+        <c:axId val="147559552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6519,7 +6548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43731200"/>
+        <c:crossAx val="147561088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6527,7 +6556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43731200"/>
+        <c:axId val="147561088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6538,7 +6567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43729664"/>
+        <c:crossAx val="147559552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6812,11 +6841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="43759104"/>
-        <c:axId val="43760640"/>
+        <c:axId val="150522112"/>
+        <c:axId val="148045824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43759104"/>
+        <c:axId val="150522112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6825,7 +6854,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43760640"/>
+        <c:crossAx val="148045824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6833,7 +6862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43760640"/>
+        <c:axId val="148045824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6844,7 +6873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43759104"/>
+        <c:crossAx val="150522112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7194,11 +7223,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44068224"/>
-        <c:axId val="44078592"/>
+        <c:axId val="147247488"/>
+        <c:axId val="147249408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44068224"/>
+        <c:axId val="147247488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7226,7 +7255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44078592"/>
+        <c:crossAx val="147249408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7234,7 +7263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44078592"/>
+        <c:axId val="147249408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7265,7 +7294,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44068224"/>
+        <c:crossAx val="147247488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7622,11 +7651,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44536192"/>
-        <c:axId val="44538112"/>
+        <c:axId val="147432576"/>
+        <c:axId val="147434496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44536192"/>
+        <c:axId val="147432576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7654,7 +7683,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44538112"/>
+        <c:crossAx val="147434496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7662,7 +7691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44538112"/>
+        <c:axId val="147434496"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7693,7 +7722,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44536192"/>
+        <c:crossAx val="147432576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7889,11 +7918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44550784"/>
-        <c:axId val="44552576"/>
+        <c:axId val="147455360"/>
+        <c:axId val="148374656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44550784"/>
+        <c:axId val="147455360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7902,7 +7931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44552576"/>
+        <c:crossAx val="148374656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7910,7 +7939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44552576"/>
+        <c:axId val="148374656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -7940,7 +7969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44550784"/>
+        <c:crossAx val="147455360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -9090,7 +9119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="B4:J13"/>
     </sheetView>
   </sheetViews>
@@ -9108,19 +9137,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
@@ -9297,60 +9326,60 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="52" t="s">
+      <c r="I11" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="J11" s="49" t="s">
+      <c r="J11" s="35" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="H12" s="49" t="s">
+      <c r="H12" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="J12" s="49" t="s">
+      <c r="J12" s="35" t="s">
         <v>107</v>
       </c>
     </row>
@@ -9384,19 +9413,19 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="39"/>
+      <c r="D16" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
@@ -11036,35 +11065,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:I37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="9" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="17" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="44" t="s">
         <v>120</v>
       </c>
@@ -11144,7 +11174,9 @@
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>123</v>
+      </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
@@ -11312,32 +11344,41 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="L10">
+        <v>96</v>
+      </c>
+      <c r="M10">
+        <v>120</v>
+      </c>
+      <c r="N10">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="44" t="str">
         <f>D3</f>
         <v>Generic C FFT</v>
@@ -11350,6 +11391,12 @@
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
       <c r="I12" s="45"/>
+      <c r="K12" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="33" t="str">
@@ -11383,6 +11430,19 @@
         <f>Summary_Speed!Q19</f>
         <v>FRDM-K66F</v>
       </c>
+      <c r="K13" s="53"/>
+      <c r="L13" s="55" t="str">
+        <f>F13</f>
+        <v>Teensy 3.2</v>
+      </c>
+      <c r="M13" s="55" t="str">
+        <f>G13</f>
+        <v>Teensy 3.5</v>
+      </c>
+      <c r="N13" s="55" t="str">
+        <f>H13</f>
+        <v>Teensy 3.6</v>
+      </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="34">
@@ -11417,10 +11477,22 @@
         <f>Summary_Speed!Q20</f>
         <v>31250</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+      <c r="K14" s="57" t="str">
+        <f>C7</f>
+        <v>Int16</v>
+      </c>
+      <c r="L14" s="58">
+        <f>F7/$F$7</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="58">
+        <f>G7/$F$7</f>
+        <v>1.3003908431044111</v>
+      </c>
+      <c r="N14" s="58">
+        <f>H7/$F$7</f>
+        <v>2.2597024579560157</v>
+      </c>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
@@ -11457,10 +11529,22 @@
         <f>Summary_Speed!Q21</f>
         <v>16666.666666666668</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="K15" s="57" t="str">
+        <f>C16</f>
+        <v>Int32</v>
+      </c>
+      <c r="L15" s="58">
+        <f>F16/$F$16</f>
+        <v>1</v>
+      </c>
+      <c r="M15" s="58">
+        <f>G16/$F$16</f>
+        <v>1.3147186147186145</v>
+      </c>
+      <c r="N15" s="58">
+        <f>H16/$F$16</f>
+        <v>2.2249084249084246</v>
+      </c>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
@@ -11497,10 +11581,22 @@
         <f>Summary_Speed!Q22</f>
         <v>6211.1801242236024</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="K16" s="57" t="str">
+        <f>C25</f>
+        <v>Float32</v>
+      </c>
+      <c r="L16" s="58">
+        <f>F25/$F$25</f>
+        <v>1</v>
+      </c>
+      <c r="M16" s="58">
+        <f>G25/$F$25</f>
+        <v>10.391963919639196</v>
+      </c>
+      <c r="N16" s="58">
+        <f>H25/$F$25</f>
+        <v>16.014743049705139</v>
+      </c>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
@@ -11537,10 +11633,21 @@
         <f>Summary_Speed!Q23</f>
         <v>3154.5741324921137</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+      <c r="K17" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="L17" s="56">
+        <f>L10/$L$10</f>
+        <v>1</v>
+      </c>
+      <c r="M17" s="56">
+        <f>M10/$L$10</f>
+        <v>1.25</v>
+      </c>
+      <c r="N17" s="56">
+        <f>N10/$L$10</f>
+        <v>1.875</v>
+      </c>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
@@ -11577,42 +11684,38 @@
         <f>Summary_Speed!Q24</f>
         <v>1272.2646310432569</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="str">
+      <c r="B21" s="43" t="str">
         <f t="shared" ref="B21:B27" si="1">B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C21" s="46"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="44" t="str">
         <f>D12</f>
         <v>Generic C FFT</v>
@@ -11862,16 +11965,16 @@
       <c r="Q27" s="10"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -11911,23 +12014,23 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="48"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="str">
+      <c r="B32" s="49" t="str">
         <f>B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C32" s="43"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="44" t="str">
         <f>D12</f>
         <v>Generic C FFT</v>
@@ -12102,25 +12205,26 @@
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:I3"/>
+  <mergeCells count="25">
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:I32"/>
     <mergeCell ref="B28:I28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:I11"/>
@@ -12133,12 +12237,12 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:I21"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:I36">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
@@ -12172,27 +12276,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="46"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="44" t="s">
         <v>59</v>
       </c>
@@ -12789,42 +12893,42 @@
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="44" t="s">
         <v>59</v>
       </c>
@@ -13424,43 +13528,43 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="str">
+      <c r="B21" s="43" t="str">
         <f t="shared" ref="B21:B27" si="15">B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C21" s="46"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="44" t="str">
         <f>D12</f>
         <v>Generic C</v>
@@ -14063,21 +14167,21 @@
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -14142,28 +14246,28 @@
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="41"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="48"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="str">
+      <c r="B32" s="49" t="str">
         <f>B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C32" s="43"/>
+      <c r="C32" s="50"/>
       <c r="D32" s="44" t="str">
         <f>D12</f>
         <v>Generic C</v>
@@ -14181,13 +14285,13 @@
       <c r="L32" s="45"/>
       <c r="M32" s="45"/>
       <c r="N32" s="45"/>
-      <c r="W32" s="38" t="s">
+      <c r="W32" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="X32" s="38"/>
-      <c r="Y32" s="38"/>
-      <c r="Z32" s="38"/>
-      <c r="AA32" s="38"/>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="42"/>
+      <c r="Z32" s="42"/>
+      <c r="AA32" s="42"/>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="str">
@@ -14509,33 +14613,24 @@
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:N31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B28:N28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="W32:AA32"/>
@@ -14552,6 +14647,15 @@
     <mergeCell ref="D20:N20"/>
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="K12:N12"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:N31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B28:N28"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:N36">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -14588,49 +14692,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="AC2" s="48" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="AC2" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="52"/>
+      <c r="AK2" s="52"/>
+      <c r="AL2" s="52"/>
+      <c r="AM2" s="52"/>
+      <c r="AN2" s="52"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="52"/>
+      <c r="AQ2" s="52"/>
     </row>
     <row r="4" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C4" t="str">
@@ -16908,58 +17012,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:53" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="AD2" s="48" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="AD2" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
-      <c r="AR2" s="48"/>
-      <c r="AS2" s="48"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48"/>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="48"/>
-      <c r="BA2" s="48"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="52"/>
+      <c r="AK2" s="52"/>
+      <c r="AL2" s="52"/>
+      <c r="AM2" s="52"/>
+      <c r="AN2" s="52"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="52"/>
+      <c r="AQ2" s="52"/>
+      <c r="AR2" s="52"/>
+      <c r="AS2" s="52"/>
+      <c r="AT2" s="52"/>
+      <c r="AU2" s="52"/>
+      <c r="AV2" s="52"/>
+      <c r="AW2" s="52"/>
+      <c r="AX2" s="52"/>
+      <c r="AY2" s="52"/>
+      <c r="AZ2" s="52"/>
+      <c r="BA2" s="52"/>
     </row>
     <row r="4" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="str">

</xml_diff>

<commit_message>
FIR_FFT Benchmarking: add ARM_RFFT and ARM_FIR
</commit_message>
<xml_diff>
--- a/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
+++ b/Arduino/Audio Processing Benchmarking/FFT Speed Results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="128">
   <si>
     <t>N</t>
   </si>
@@ -402,6 +402,18 @@
   <si>
     <t>s</t>
   </si>
+  <si>
+    <t>RFFT</t>
+  </si>
+  <si>
+    <t>FFTs Per Second</t>
+  </si>
+  <si>
+    <t>CFFT Radix 4</t>
+  </si>
+  <si>
+    <t>CFFT Radix 2</t>
+  </si>
 </sst>
 </file>
 
@@ -543,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -612,12 +624,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -689,25 +710,28 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -725,24 +749,34 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="10" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -939,11 +973,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147113088"/>
-        <c:axId val="147114624"/>
+        <c:axId val="253647488"/>
+        <c:axId val="253665664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147113088"/>
+        <c:axId val="253647488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,7 +986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147114624"/>
+        <c:crossAx val="253665664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -960,7 +994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147114624"/>
+        <c:axId val="253665664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +1005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147113088"/>
+        <c:crossAx val="253647488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1098,11 +1132,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148399616"/>
-        <c:axId val="148401152"/>
+        <c:axId val="255036032"/>
+        <c:axId val="255041920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148399616"/>
+        <c:axId val="255036032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1113,12 +1147,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148401152"/>
+        <c:crossAx val="255041920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148401152"/>
+        <c:axId val="255041920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1130,7 +1164,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148399616"/>
+        <c:crossAx val="255036032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1407,11 +1441,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148422016"/>
-        <c:axId val="148444288"/>
+        <c:axId val="254870272"/>
+        <c:axId val="254871808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148422016"/>
+        <c:axId val="254870272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148444288"/>
+        <c:crossAx val="254871808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148444288"/>
+        <c:axId val="254871808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -1466,7 +1500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148422016"/>
+        <c:crossAx val="254870272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1695,11 +1729,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148482304"/>
-        <c:axId val="148488192"/>
+        <c:axId val="254918016"/>
+        <c:axId val="254919808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148482304"/>
+        <c:axId val="254918016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148488192"/>
+        <c:crossAx val="254919808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148488192"/>
+        <c:axId val="254919808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,7 +1796,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148482304"/>
+        <c:crossAx val="254918016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2216,11 +2250,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="148248448"/>
-        <c:axId val="148249984"/>
+        <c:axId val="254958592"/>
+        <c:axId val="254976768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148248448"/>
+        <c:axId val="254958592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +2263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148249984"/>
+        <c:crossAx val="254976768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2237,7 +2271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148249984"/>
+        <c:axId val="254976768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2266,7 +2300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148248448"/>
+        <c:crossAx val="254958592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -2318,6 +2352,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2671,11 +2706,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147910016"/>
-        <c:axId val="147789312"/>
+        <c:axId val="255173376"/>
+        <c:axId val="255175296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147910016"/>
+        <c:axId val="255173376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,13 +2732,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147789312"/>
+        <c:crossAx val="255175296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2711,7 +2747,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147789312"/>
+        <c:axId val="255175296"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2737,19 +2773,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147910016"/>
+        <c:crossAx val="255173376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2794,6 +2832,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3147,11 +3186,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147821696"/>
-        <c:axId val="147823616"/>
+        <c:axId val="255539456"/>
+        <c:axId val="255553920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147821696"/>
+        <c:axId val="255539456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3173,13 +3212,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147823616"/>
+        <c:crossAx val="255553920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3187,7 +3227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147823616"/>
+        <c:axId val="255553920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3213,19 +3253,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147821696"/>
+        <c:crossAx val="255539456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3498,11 +3540,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148296832"/>
-        <c:axId val="148298752"/>
+        <c:axId val="255265024"/>
+        <c:axId val="255271296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148296832"/>
+        <c:axId val="255265024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3530,7 +3572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148298752"/>
+        <c:crossAx val="255271296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3538,7 +3580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148298752"/>
+        <c:axId val="255271296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3567,7 +3609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148296832"/>
+        <c:crossAx val="255265024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3846,11 +3888,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148014208"/>
-        <c:axId val="148016128"/>
+        <c:axId val="255314176"/>
+        <c:axId val="255320448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148014208"/>
+        <c:axId val="255314176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3878,7 +3920,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148016128"/>
+        <c:crossAx val="255320448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3886,7 +3928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148016128"/>
+        <c:axId val="255320448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3915,7 +3957,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148014208"/>
+        <c:crossAx val="255314176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4194,11 +4236,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148771968"/>
-        <c:axId val="148773888"/>
+        <c:axId val="255351040"/>
+        <c:axId val="255369600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148771968"/>
+        <c:axId val="255351040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4226,7 +4268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148773888"/>
+        <c:crossAx val="255369600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4234,7 +4276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148773888"/>
+        <c:axId val="255369600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4263,7 +4305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148771968"/>
+        <c:crossAx val="255351040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4524,11 +4566,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148817024"/>
-        <c:axId val="148818944"/>
+        <c:axId val="255461632"/>
+        <c:axId val="255467904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148817024"/>
+        <c:axId val="255461632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4556,7 +4598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148818944"/>
+        <c:crossAx val="255467904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4564,7 +4606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148818944"/>
+        <c:axId val="255467904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4593,7 +4635,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148817024"/>
+        <c:crossAx val="255461632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4820,11 +4862,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147479936"/>
-        <c:axId val="147481728"/>
+        <c:axId val="254089856"/>
+        <c:axId val="254099840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147479936"/>
+        <c:axId val="254089856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4833,7 +4875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147481728"/>
+        <c:crossAx val="254099840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4841,7 +4883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147481728"/>
+        <c:axId val="254099840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4852,7 +4894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147479936"/>
+        <c:crossAx val="254089856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5114,11 +5156,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="148845696"/>
-        <c:axId val="148847616"/>
+        <c:axId val="255498496"/>
+        <c:axId val="255508864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148845696"/>
+        <c:axId val="255498496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5146,7 +5188,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148847616"/>
+        <c:crossAx val="255508864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5154,7 +5196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148847616"/>
+        <c:axId val="255508864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5183,7 +5225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148845696"/>
+        <c:crossAx val="255498496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5444,11 +5486,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="153429504"/>
-        <c:axId val="153431424"/>
+        <c:axId val="255871616"/>
+        <c:axId val="255877888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="153429504"/>
+        <c:axId val="255871616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5476,7 +5518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153431424"/>
+        <c:crossAx val="255877888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5484,7 +5526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153431424"/>
+        <c:axId val="255877888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5513,7 +5555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153429504"/>
+        <c:crossAx val="255871616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5573,6 +5615,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6039,11 +6082,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147646720"/>
-        <c:axId val="147521920"/>
+        <c:axId val="254178432"/>
+        <c:axId val="254180352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147646720"/>
+        <c:axId val="254178432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6065,13 +6108,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147521920"/>
+        <c:crossAx val="254180352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6079,7 +6123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147521920"/>
+        <c:axId val="254180352"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6104,13 +6148,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147646720"/>
+        <c:crossAx val="254178432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6190,6 +6235,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6277,11 +6323,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144329344"/>
-        <c:axId val="146694528"/>
+        <c:axId val="254480384"/>
+        <c:axId val="254481920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144329344"/>
+        <c:axId val="254480384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6290,7 +6336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146694528"/>
+        <c:crossAx val="254481920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6298,7 +6344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146694528"/>
+        <c:axId val="254481920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6309,13 +6355,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144329344"/>
+        <c:crossAx val="254480384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6535,11 +6582,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147559552"/>
-        <c:axId val="147561088"/>
+        <c:axId val="254499456"/>
+        <c:axId val="254505344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147559552"/>
+        <c:axId val="254499456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6548,7 +6595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147561088"/>
+        <c:crossAx val="254505344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6556,7 +6603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147561088"/>
+        <c:axId val="254505344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6567,7 +6614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147559552"/>
+        <c:crossAx val="254499456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6841,11 +6888,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150522112"/>
-        <c:axId val="148045824"/>
+        <c:axId val="254528512"/>
+        <c:axId val="254292736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150522112"/>
+        <c:axId val="254528512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6854,7 +6901,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148045824"/>
+        <c:crossAx val="254292736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6862,7 +6909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148045824"/>
+        <c:axId val="254292736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6873,7 +6920,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150522112"/>
+        <c:crossAx val="254528512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6925,6 +6972,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7223,11 +7271,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147247488"/>
-        <c:axId val="147249408"/>
+        <c:axId val="254461056"/>
+        <c:axId val="254462976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147247488"/>
+        <c:axId val="254461056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7249,13 +7297,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147249408"/>
+        <c:crossAx val="254462976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7263,7 +7312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147249408"/>
+        <c:axId val="254462976"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7288,19 +7337,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147247488"/>
+        <c:crossAx val="254461056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7353,6 +7404,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7651,11 +7703,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="147432576"/>
-        <c:axId val="147434496"/>
+        <c:axId val="254642048"/>
+        <c:axId val="254656512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="147432576"/>
+        <c:axId val="254642048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7677,13 +7729,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147434496"/>
+        <c:crossAx val="254656512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7691,7 +7744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="147434496"/>
+        <c:axId val="254656512"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7716,19 +7769,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147432576"/>
+        <c:crossAx val="254642048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7918,11 +7973,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="147455360"/>
-        <c:axId val="148374656"/>
+        <c:axId val="255013632"/>
+        <c:axId val="255015168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="147455360"/>
+        <c:axId val="255013632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7931,7 +7986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148374656"/>
+        <c:crossAx val="255015168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7939,7 +7994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148374656"/>
+        <c:axId val="255015168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -7969,7 +8024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147455360"/>
+        <c:crossAx val="255013632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2000"/>
@@ -9125,31 +9180,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="9.625" customWidth="1"/>
+    <col min="8" max="8" width="7.875" customWidth="1"/>
+    <col min="9" max="9" width="5.25" customWidth="1"/>
+    <col min="10" max="10" width="7.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
@@ -9413,19 +9468,19 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40" t="s">
+      <c r="C16" s="45"/>
+      <c r="D16" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
@@ -11065,46 +11120,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="9" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="17" width="9.140625" customWidth="1"/>
+    <col min="2" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="9" width="12.75" customWidth="1"/>
+    <col min="10" max="10" width="10.75" style="60" customWidth="1"/>
+    <col min="11" max="11" width="12.75" customWidth="1"/>
+    <col min="12" max="14" width="11.375" customWidth="1"/>
+    <col min="15" max="17" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="33" t="str">
@@ -11344,14 +11400,14 @@
       <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
       <c r="L10">
         <v>96</v>
       </c>
@@ -11363,40 +11419,40 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42" t="s">
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44" t="str">
+      <c r="C12" s="56"/>
+      <c r="D12" s="54" t="str">
         <f>D3</f>
         <v>Generic C FFT</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="45" t="str">
+      <c r="E12" s="54"/>
+      <c r="F12" s="55" t="str">
         <f>F3</f>
         <v>CMSIS FFT</v>
       </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="K12" s="42" t="s">
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="K12" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="33" t="str">
@@ -11430,16 +11486,16 @@
         <f>Summary_Speed!Q19</f>
         <v>FRDM-K66F</v>
       </c>
-      <c r="K13" s="53"/>
-      <c r="L13" s="55" t="str">
+      <c r="K13" s="39"/>
+      <c r="L13" s="41" t="str">
         <f>F13</f>
         <v>Teensy 3.2</v>
       </c>
-      <c r="M13" s="55" t="str">
+      <c r="M13" s="41" t="str">
         <f>G13</f>
         <v>Teensy 3.5</v>
       </c>
-      <c r="N13" s="55" t="str">
+      <c r="N13" s="41" t="str">
         <f>H13</f>
         <v>Teensy 3.6</v>
       </c>
@@ -11477,19 +11533,19 @@
         <f>Summary_Speed!Q20</f>
         <v>31250</v>
       </c>
-      <c r="K14" s="57" t="str">
+      <c r="K14" s="43" t="str">
         <f>C7</f>
         <v>Int16</v>
       </c>
-      <c r="L14" s="58">
+      <c r="L14" s="44">
         <f>F7/$F$7</f>
         <v>1</v>
       </c>
-      <c r="M14" s="58">
+      <c r="M14" s="44">
         <f>G7/$F$7</f>
         <v>1.3003908431044111</v>
       </c>
-      <c r="N14" s="58">
+      <c r="N14" s="44">
         <f>H7/$F$7</f>
         <v>2.2597024579560157</v>
       </c>
@@ -11529,19 +11585,19 @@
         <f>Summary_Speed!Q21</f>
         <v>16666.666666666668</v>
       </c>
-      <c r="K15" s="57" t="str">
+      <c r="K15" s="43" t="str">
         <f>C16</f>
         <v>Int32</v>
       </c>
-      <c r="L15" s="58">
+      <c r="L15" s="44">
         <f>F16/$F$16</f>
         <v>1</v>
       </c>
-      <c r="M15" s="58">
+      <c r="M15" s="44">
         <f>G16/$F$16</f>
         <v>1.3147186147186145</v>
       </c>
-      <c r="N15" s="58">
+      <c r="N15" s="44">
         <f>H16/$F$16</f>
         <v>2.2249084249084246</v>
       </c>
@@ -11581,19 +11637,19 @@
         <f>Summary_Speed!Q22</f>
         <v>6211.1801242236024</v>
       </c>
-      <c r="K16" s="57" t="str">
+      <c r="K16" s="43" t="str">
         <f>C25</f>
         <v>Float32</v>
       </c>
-      <c r="L16" s="58">
+      <c r="L16" s="44">
         <f>F25/$F$25</f>
         <v>1</v>
       </c>
-      <c r="M16" s="58">
+      <c r="M16" s="44">
         <f>G25/$F$25</f>
         <v>10.391963919639196</v>
       </c>
-      <c r="N16" s="58">
+      <c r="N16" s="44">
         <f>H25/$F$25</f>
         <v>16.014743049705139</v>
       </c>
@@ -11633,18 +11689,18 @@
         <f>Summary_Speed!Q23</f>
         <v>3154.5741324921137</v>
       </c>
-      <c r="K17" s="54" t="s">
+      <c r="K17" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="56">
+      <c r="L17" s="42">
         <f>L10/$L$10</f>
         <v>1</v>
       </c>
-      <c r="M17" s="56">
+      <c r="M17" s="42">
         <f>M10/$L$10</f>
         <v>1.25</v>
       </c>
-      <c r="N17" s="56">
+      <c r="N17" s="42">
         <f>N10/$L$10</f>
         <v>1.875</v>
       </c>
@@ -11689,45 +11745,57 @@
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="K20" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="str">
+      <c r="B21" s="56" t="str">
         <f t="shared" ref="B21:B27" si="1">B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44" t="str">
+      <c r="C21" s="56"/>
+      <c r="D21" s="54" t="str">
         <f>D12</f>
         <v>Generic C FFT</v>
       </c>
-      <c r="E21" s="44"/>
-      <c r="F21" s="45" t="str">
+      <c r="E21" s="54"/>
+      <c r="F21" s="55" t="str">
         <f>F12</f>
         <v>CMSIS FFT</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="K21" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="O21" t="s">
+        <v>2</v>
+      </c>
+      <c r="P21" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="33" t="str">
@@ -11762,6 +11830,27 @@
         <f t="shared" si="2"/>
         <v>FRDM-K66F</v>
       </c>
+      <c r="K22" s="62" t="str">
+        <f>O22</f>
+        <v>RFFT</v>
+      </c>
+      <c r="L22" s="62" t="str">
+        <f t="shared" ref="L22:M22" si="3">P22</f>
+        <v>CFFT Radix 4</v>
+      </c>
+      <c r="M22" s="62" t="str">
+        <f t="shared" si="3"/>
+        <v>CFFT Radix 2</v>
+      </c>
+      <c r="O22" t="s">
+        <v>124</v>
+      </c>
+      <c r="P22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="34">
@@ -11796,13 +11885,27 @@
         <f>Summary_Speed!Y20</f>
         <v>40000</v>
       </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
+      <c r="K23" s="17">
+        <f>1000000/O23</f>
+        <v>63451.776649746193</v>
+      </c>
+      <c r="L23" s="17">
+        <f t="shared" ref="L23:M27" si="4">1000000/P23</f>
+        <v>48971.596474045051</v>
+      </c>
+      <c r="M23" s="17">
+        <f t="shared" si="4"/>
+        <v>38284.839203675343</v>
+      </c>
+      <c r="O23" s="59">
+        <v>15.76</v>
+      </c>
+      <c r="P23" s="63">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="Q23" s="63">
+        <v>26.12</v>
+      </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="34">
@@ -11836,13 +11939,27 @@
         <f>Summary_Speed!Y21</f>
         <v>21276.59574468085</v>
       </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
+      <c r="K24" s="17">
+        <f>1000000/O24</f>
+        <v>28169.014084507042</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" si="4"/>
+        <v>24826.216484607747</v>
+      </c>
+      <c r="M24" s="17">
+        <f t="shared" si="4"/>
+        <v>16886.187098953058</v>
+      </c>
+      <c r="O24" s="59">
+        <v>35.5</v>
+      </c>
+      <c r="P24" s="63">
+        <v>40.28</v>
+      </c>
+      <c r="Q24" s="63">
+        <v>59.22</v>
+      </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="34">
@@ -11876,13 +11993,27 @@
         <f>Summary_Speed!Y22</f>
         <v>9523.8095238095229</v>
       </c>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="K25" s="17">
+        <f>1000000/O25</f>
+        <v>14355.44071202986</v>
+      </c>
+      <c r="L25" s="17">
+        <f t="shared" si="4"/>
+        <v>10506.408909434755</v>
+      </c>
+      <c r="M25" s="17">
+        <f t="shared" si="4"/>
+        <v>7602.2502660787595</v>
+      </c>
+      <c r="O25" s="59">
+        <v>69.66</v>
+      </c>
+      <c r="P25" s="63">
+        <v>95.18</v>
+      </c>
+      <c r="Q25" s="63">
+        <v>131.54</v>
+      </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="34">
@@ -11916,13 +12047,27 @@
         <f>Summary_Speed!Y23</f>
         <v>4878.0487804878048</v>
       </c>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
+      <c r="K26" s="17">
+        <f>1000000/O26</f>
+        <v>6397.9526551503513</v>
+      </c>
+      <c r="L26" s="17">
+        <f t="shared" si="4"/>
+        <v>5236.1503822389786</v>
+      </c>
+      <c r="M26" s="17">
+        <f t="shared" si="4"/>
+        <v>3433.8300940869444</v>
+      </c>
+      <c r="O26" s="59">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="P26" s="63">
+        <v>190.98</v>
+      </c>
+      <c r="Q26" s="63">
+        <v>291.22000000000003</v>
+      </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="34">
@@ -11956,25 +12101,39 @@
         <f>Summary_Speed!Y24</f>
         <v>2123.1422505307855</v>
       </c>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
+      <c r="K27" s="17">
+        <f>1000000/O27</f>
+        <v>3245.4887706088534</v>
+      </c>
+      <c r="L27" s="17">
+        <f t="shared" si="4"/>
+        <v>2497.5024975024976</v>
+      </c>
+      <c r="M27" s="17">
+        <f t="shared" si="4"/>
+        <v>1567.2998558084134</v>
+      </c>
+      <c r="O27" s="59">
+        <v>308.12</v>
+      </c>
+      <c r="P27" s="63">
+        <v>400.4</v>
+      </c>
+      <c r="Q27" s="63">
+        <v>638.04</v>
+      </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -11985,6 +12144,14 @@
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
+      <c r="O29">
+        <f>O23/P23</f>
+        <v>0.77179236043095001</v>
+      </c>
+      <c r="Q29">
+        <f>P23/Q23</f>
+        <v>0.78177641653905061</v>
+      </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
@@ -11997,54 +12164,78 @@
         <v>4</v>
       </c>
       <c r="F30" s="15">
-        <f t="shared" ref="F30:I30" si="3">E30+1</f>
+        <f t="shared" ref="F30:H30" si="5">E30+1</f>
         <v>5</v>
       </c>
       <c r="G30" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="H30" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="I30" s="15">
-        <f t="shared" si="3"/>
+        <f>H30+1</f>
         <v>8</v>
       </c>
+      <c r="O30">
+        <f t="shared" ref="O30:O33" si="6">O24/P24</f>
+        <v>0.88133068520357494</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" ref="Q30:Q33" si="7">P24/Q24</f>
+        <v>0.68017561634582913</v>
+      </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="46" t="s">
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="48"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="51"/>
+      <c r="O31">
+        <f t="shared" si="6"/>
+        <v>0.73187644463122492</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="7"/>
+        <v>0.72358218032537636</v>
+      </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="str">
+      <c r="B32" s="52" t="str">
         <f>B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="44" t="str">
+      <c r="C32" s="53"/>
+      <c r="D32" s="54" t="str">
         <f>D12</f>
         <v>Generic C FFT</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="45" t="str">
+      <c r="E32" s="54"/>
+      <c r="F32" s="55" t="str">
         <f>F12</f>
         <v>CMSIS FFT</v>
       </c>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="O32">
+        <f t="shared" si="6"/>
+        <v>0.81841030474395238</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="7"/>
+        <v>0.65579287136872455</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="33" t="str">
         <f>B22</f>
         <v>N</v>
@@ -12058,23 +12249,23 @@
         <v>Arduino Uno</v>
       </c>
       <c r="E33" s="33" t="str">
-        <f t="shared" ref="E33:I33" si="4">E13</f>
+        <f t="shared" ref="E33:I33" si="8">E13</f>
         <v>Arduino M0</v>
       </c>
       <c r="F33" s="33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Teensy 3.2</v>
       </c>
       <c r="G33" s="33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Teensy 3.5</v>
       </c>
       <c r="H33" s="33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>Teensy 3.6</v>
       </c>
       <c r="I33" s="33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>FRDM-K66F</v>
       </c>
       <c r="K33" t="s">
@@ -12083,8 +12274,16 @@
       <c r="L33" s="19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <f t="shared" si="6"/>
+        <v>0.76953046953046955</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="7"/>
+        <v>0.62754686226568868</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="34">
         <f>B7</f>
         <v>128</v>
@@ -12124,7 +12323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="34">
         <f>B16</f>
         <v>128</v>
@@ -12164,7 +12363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="34">
         <f>B25</f>
         <v>128</v>
@@ -12204,20 +12403,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:I12"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="B37:I37"/>
     <mergeCell ref="B31:C31"/>
@@ -12226,23 +12436,12 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:I12"/>
     <mergeCell ref="B19:I19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:I20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:I21"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:I3"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:I36">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
@@ -12253,7 +12452,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12261,57 +12461,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="D31" sqref="D31:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="14" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="17" max="22" width="9.140625" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="7.25" customWidth="1"/>
+    <col min="4" max="14" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="10.625" customWidth="1"/>
+    <col min="17" max="22" width="9.125" customWidth="1"/>
+    <col min="23" max="23" width="11.875" customWidth="1"/>
     <col min="24" max="27" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="str">
@@ -12893,57 +13093,57 @@
       </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42" t="s">
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="45" t="s">
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="str">
@@ -13528,60 +13728,60 @@
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="str">
+      <c r="B21" s="56" t="str">
         <f t="shared" ref="B21:B27" si="15">B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44" t="str">
+      <c r="C21" s="56"/>
+      <c r="D21" s="54" t="str">
         <f>D12</f>
         <v>Generic C</v>
       </c>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="45" t="str">
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="55" t="str">
         <f>K12</f>
         <v>CMSIS</v>
       </c>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="str">
@@ -14167,21 +14367,21 @@
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
@@ -14246,52 +14446,52 @@
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="46" t="s">
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="48"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="51"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="str">
+      <c r="B32" s="52" t="str">
         <f>B12</f>
         <v>Inputs</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="44" t="str">
+      <c r="C32" s="53"/>
+      <c r="D32" s="54" t="str">
         <f>D12</f>
         <v>Generic C</v>
       </c>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="45" t="str">
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="55" t="str">
         <f>K12</f>
         <v>CMSIS</v>
       </c>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="W32" s="42" t="s">
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
+      <c r="N32" s="55"/>
+      <c r="W32" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
-      <c r="Z32" s="42"/>
-      <c r="AA32" s="42"/>
+      <c r="X32" s="47"/>
+      <c r="Y32" s="47"/>
+      <c r="Z32" s="47"/>
+      <c r="AA32" s="47"/>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="str">
@@ -14613,24 +14813,33 @@
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:N31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B28:N28"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="W32:AA32"/>
@@ -14647,15 +14856,6 @@
     <mergeCell ref="D20:N20"/>
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="K12:N12"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:N31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B28:N28"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:N36">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -14675,66 +14875,66 @@
   <dimension ref="B2:AQ38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AK33" sqref="AK33:AL36"/>
+      <selection activeCell="G26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="3" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" customWidth="1"/>
-    <col min="11" max="17" width="10.140625" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="3" max="9" width="10.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="17" width="10.125" customWidth="1"/>
+    <col min="18" max="18" width="3.375" customWidth="1"/>
+    <col min="23" max="23" width="10.125" customWidth="1"/>
     <col min="27" max="27" width="3" style="14" customWidth="1"/>
-    <col min="28" max="28" width="11.28515625" customWidth="1"/>
-    <col min="34" max="34" width="10.140625" customWidth="1"/>
+    <col min="28" max="28" width="11.25" customWidth="1"/>
+    <col min="34" max="34" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="AC2" s="52" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="AC2" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="52"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
     </row>
     <row r="4" spans="2:43" x14ac:dyDescent="0.25">
       <c r="C4" t="str">
@@ -15691,22 +15891,6 @@
       <c r="S18" t="str">
         <f>C18</f>
         <v>FFT per sec</v>
-      </c>
-      <c r="V18" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="W18" t="str">
-        <f>'Teensy 3.2'!$C$2</f>
-        <v>Teensy 3.2</v>
-      </c>
-      <c r="X18" t="str">
-        <f>'Teensy 3.5'!C2</f>
-        <v>Teensy 3.5</v>
-      </c>
-      <c r="Y18" t="str">
-        <f>'NXP K66'!$C$2</f>
-        <v>FRDM-K66F</v>
       </c>
       <c r="AC18" t="str">
         <f>'Summary-Duration'!AE5</f>
@@ -17003,67 +17187,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="3" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" customWidth="1"/>
-    <col min="11" max="17" width="10.140625" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="2"/>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="3" max="9" width="10.875" customWidth="1"/>
+    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="11" max="17" width="10.125" customWidth="1"/>
+    <col min="18" max="18" width="3.375" customWidth="1"/>
+    <col min="28" max="28" width="9.125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:53" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="AD2" s="52" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+      <c r="AD2" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="52"/>
-      <c r="AR2" s="52"/>
-      <c r="AS2" s="52"/>
-      <c r="AT2" s="52"/>
-      <c r="AU2" s="52"/>
-      <c r="AV2" s="52"/>
-      <c r="AW2" s="52"/>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="52"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="58"/>
     </row>
     <row r="4" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="str">
@@ -19357,12 +19541,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" customWidth="1"/>
+    <col min="6" max="6" width="10.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>